<commit_message>
Added opdracht template.xlsx Changed grondwater_template.xlsx to not include filterdebietmeter
</commit_message>
<xml_diff>
--- a/data/grondwater_template.xlsx
+++ b/data/grondwater_template.xlsx
@@ -11,15 +11,14 @@
     <sheet name="grondwaterlocatie" sheetId="2" r:id="rId2"/>
     <sheet name="filter" sheetId="3" r:id="rId3"/>
     <sheet name="filtermeting" sheetId="4" r:id="rId4"/>
-    <sheet name="filterdebietmeter" sheetId="5" r:id="rId5"/>
-    <sheet name="opdracht" sheetId="6" r:id="rId6"/>
+    <sheet name="opdracht" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8515" uniqueCount="3080">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8473" uniqueCount="3070">
   <si>
     <t>identificatie</t>
   </si>
@@ -8986,36 +8985,6 @@
   </si>
   <si>
     <t>filtermeting</t>
-  </si>
-  <si>
-    <t>debietmeter-serienummer</t>
-  </si>
-  <si>
-    <t>serienummer</t>
-  </si>
-  <si>
-    <t>debietmeter-merk</t>
-  </si>
-  <si>
-    <t>merk</t>
-  </si>
-  <si>
-    <t>debietmeter-datum_ijking</t>
-  </si>
-  <si>
-    <t>datum_ijking</t>
-  </si>
-  <si>
-    <t>debietmeter-datum_wegname</t>
-  </si>
-  <si>
-    <t>datum_wegname</t>
-  </si>
-  <si>
-    <t>debietmeter</t>
-  </si>
-  <si>
-    <t>filterdebietmeter</t>
   </si>
   <si>
     <t>opdrachtgever-choice_1-naam</t>
@@ -9953,7 +9922,7 @@
 </file>
 
 <file path=xl/tables/table63.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="63" name="Table63" displayName="Table63" ref="DU3:DV10" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="63" name="Table63" displayName="Table63" ref="DU3:DV8" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -9963,7 +9932,7 @@
 </file>
 
 <file path=xl/tables/table64.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="64" name="Table64" displayName="Table64" ref="DW3:DX8" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="64" name="Table64" displayName="Table64" ref="DW3:DX17" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -9973,7 +9942,7 @@
 </file>
 
 <file path=xl/tables/table65.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="65" name="Table65" displayName="Table65" ref="DY3:DZ17" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="65" name="Table65" displayName="Table65" ref="DY3:DZ27" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -9983,17 +9952,7 @@
 </file>
 
 <file path=xl/tables/table66.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="66" name="Table66" displayName="Table66" ref="EA3:EB27" totalsRowShown="0">
-  <tableColumns count="2">
-    <tableColumn id="1" name="Code"/>
-    <tableColumn id="2" name="Beschrijving"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="1"/>
-</table>
-</file>
-
-<file path=xl/tables/table67.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="67" name="Table67" displayName="Table67" ref="EC3:ED60" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="66" name="Table66" displayName="Table66" ref="EA3:EB60" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -10317,16 +10276,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:ED918"/>
+  <dimension ref="A1:EB918"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="135" width="10.7109375" customWidth="1"/>
+    <col min="1" max="133" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:134">
+    <row r="1" spans="1:132">
       <c r="A1" s="1" t="s">
         <v>1007</v>
       </c>
@@ -10458,21 +10417,17 @@
       <c r="DS1" s="1"/>
       <c r="DT1" s="1"/>
       <c r="DU1" s="1" t="s">
-        <v>2998</v>
+        <v>152</v>
       </c>
       <c r="DV1" s="1"/>
-      <c r="DW1" s="1" t="s">
-        <v>152</v>
-      </c>
+      <c r="DW1" s="1"/>
       <c r="DX1" s="1"/>
       <c r="DY1" s="1"/>
       <c r="DZ1" s="1"/>
       <c r="EA1" s="1"/>
       <c r="EB1" s="1"/>
-      <c r="EC1" s="1"/>
-      <c r="ED1" s="1"/>
-    </row>
-    <row r="2" spans="1:134">
+    </row>
+    <row r="2" spans="1:132">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -10722,27 +10677,23 @@
       </c>
       <c r="DT2" s="1"/>
       <c r="DU2" s="1" t="s">
-        <v>1569</v>
+        <v>153</v>
       </c>
       <c r="DV2" s="1"/>
       <c r="DW2" s="1" t="s">
-        <v>153</v>
+        <v>3029</v>
       </c>
       <c r="DX2" s="1"/>
       <c r="DY2" s="1" t="s">
-        <v>3039</v>
+        <v>3031</v>
       </c>
       <c r="DZ2" s="1"/>
       <c r="EA2" s="1" t="s">
-        <v>3041</v>
+        <v>166</v>
       </c>
       <c r="EB2" s="1"/>
-      <c r="EC2" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="ED2" s="1"/>
-    </row>
-    <row r="3" spans="1:134">
+    </row>
+    <row r="3" spans="1:132">
       <c r="A3" t="s">
         <v>174</v>
       </c>
@@ -11139,14 +11090,8 @@
       <c r="EB3" t="s">
         <v>175</v>
       </c>
-      <c r="EC3" t="s">
-        <v>174</v>
-      </c>
-      <c r="ED3" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:134">
+    </row>
+    <row r="4" spans="1:132">
       <c r="A4" t="s">
         <v>171</v>
       </c>
@@ -11520,37 +11465,31 @@
         <v>172</v>
       </c>
       <c r="DU4" t="s">
-        <v>1061</v>
+        <v>945</v>
       </c>
       <c r="DV4" t="s">
         <v>172</v>
       </c>
       <c r="DW4" t="s">
-        <v>945</v>
+        <v>3034</v>
       </c>
       <c r="DX4" t="s">
         <v>172</v>
       </c>
       <c r="DY4" t="s">
-        <v>3044</v>
+        <v>3047</v>
       </c>
       <c r="DZ4" t="s">
         <v>172</v>
       </c>
       <c r="EA4" t="s">
-        <v>3057</v>
+        <v>950</v>
       </c>
       <c r="EB4" t="s">
         <v>172</v>
       </c>
-      <c r="EC4" t="s">
-        <v>950</v>
-      </c>
-      <c r="ED4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:134">
+    </row>
+    <row r="5" spans="1:132">
       <c r="A5" t="s">
         <v>173</v>
       </c>
@@ -11924,37 +11863,31 @@
         <v>172</v>
       </c>
       <c r="DU5" t="s">
-        <v>1062</v>
+        <v>946</v>
       </c>
       <c r="DV5" t="s">
         <v>172</v>
       </c>
       <c r="DW5" t="s">
-        <v>946</v>
+        <v>3035</v>
       </c>
       <c r="DX5" t="s">
         <v>172</v>
       </c>
       <c r="DY5" t="s">
-        <v>3045</v>
+        <v>3048</v>
       </c>
       <c r="DZ5" t="s">
         <v>172</v>
       </c>
       <c r="EA5" t="s">
-        <v>3058</v>
+        <v>951</v>
       </c>
       <c r="EB5" t="s">
         <v>172</v>
       </c>
-      <c r="EC5" t="s">
-        <v>951</v>
-      </c>
-      <c r="ED5" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:134">
+    </row>
+    <row r="6" spans="1:132">
       <c r="C6" t="s">
         <v>178</v>
       </c>
@@ -12316,37 +12249,31 @@
         <v>172</v>
       </c>
       <c r="DU6" t="s">
-        <v>1063</v>
+        <v>947</v>
       </c>
       <c r="DV6" t="s">
         <v>172</v>
       </c>
       <c r="DW6" t="s">
-        <v>947</v>
+        <v>3036</v>
       </c>
       <c r="DX6" t="s">
         <v>172</v>
       </c>
       <c r="DY6" t="s">
-        <v>3046</v>
+        <v>3049</v>
       </c>
       <c r="DZ6" t="s">
         <v>172</v>
       </c>
       <c r="EA6" t="s">
-        <v>3059</v>
+        <v>952</v>
       </c>
       <c r="EB6" t="s">
         <v>172</v>
       </c>
-      <c r="EC6" t="s">
-        <v>952</v>
-      </c>
-      <c r="ED6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="7" spans="1:134">
+    </row>
+    <row r="7" spans="1:132">
       <c r="C7" t="s">
         <v>179</v>
       </c>
@@ -12624,37 +12551,31 @@
         <v>172</v>
       </c>
       <c r="DU7" t="s">
-        <v>1064</v>
+        <v>948</v>
       </c>
       <c r="DV7" t="s">
         <v>172</v>
       </c>
       <c r="DW7" t="s">
-        <v>948</v>
+        <v>3037</v>
       </c>
       <c r="DX7" t="s">
         <v>172</v>
       </c>
       <c r="DY7" t="s">
-        <v>3047</v>
+        <v>3050</v>
       </c>
       <c r="DZ7" t="s">
         <v>172</v>
       </c>
       <c r="EA7" t="s">
-        <v>3060</v>
+        <v>953</v>
       </c>
       <c r="EB7" t="s">
         <v>172</v>
       </c>
-      <c r="EC7" t="s">
-        <v>953</v>
-      </c>
-      <c r="ED7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:134">
+    </row>
+    <row r="8" spans="1:132">
       <c r="C8" t="s">
         <v>180</v>
       </c>
@@ -12914,37 +12835,31 @@
         <v>172</v>
       </c>
       <c r="DU8" t="s">
-        <v>1065</v>
+        <v>949</v>
       </c>
       <c r="DV8" t="s">
         <v>172</v>
       </c>
       <c r="DW8" t="s">
-        <v>949</v>
+        <v>3038</v>
       </c>
       <c r="DX8" t="s">
         <v>172</v>
       </c>
       <c r="DY8" t="s">
-        <v>3048</v>
+        <v>3051</v>
       </c>
       <c r="DZ8" t="s">
         <v>172</v>
       </c>
       <c r="EA8" t="s">
-        <v>3061</v>
+        <v>954</v>
       </c>
       <c r="EB8" t="s">
         <v>172</v>
       </c>
-      <c r="EC8" t="s">
-        <v>954</v>
-      </c>
-      <c r="ED8" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="9" spans="1:134">
+    </row>
+    <row r="9" spans="1:132">
       <c r="C9" t="s">
         <v>181</v>
       </c>
@@ -13173,32 +13088,26 @@
       <c r="DP9" t="s">
         <v>172</v>
       </c>
-      <c r="DU9" t="s">
-        <v>1066</v>
-      </c>
-      <c r="DV9" t="s">
+      <c r="DW9" t="s">
+        <v>3039</v>
+      </c>
+      <c r="DX9" t="s">
         <v>172</v>
       </c>
       <c r="DY9" t="s">
-        <v>3049</v>
+        <v>3052</v>
       </c>
       <c r="DZ9" t="s">
         <v>172</v>
       </c>
       <c r="EA9" t="s">
-        <v>3062</v>
+        <v>955</v>
       </c>
       <c r="EB9" t="s">
         <v>172</v>
       </c>
-      <c r="EC9" t="s">
-        <v>955</v>
-      </c>
-      <c r="ED9" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:134">
+    </row>
+    <row r="10" spans="1:132">
       <c r="C10" t="s">
         <v>182</v>
       </c>
@@ -13415,32 +13324,26 @@
       <c r="DP10" t="s">
         <v>172</v>
       </c>
-      <c r="DU10" t="s">
-        <v>1067</v>
-      </c>
-      <c r="DV10" t="s">
+      <c r="DW10" t="s">
+        <v>3040</v>
+      </c>
+      <c r="DX10" t="s">
         <v>172</v>
       </c>
       <c r="DY10" t="s">
-        <v>3050</v>
+        <v>3053</v>
       </c>
       <c r="DZ10" t="s">
         <v>172</v>
       </c>
       <c r="EA10" t="s">
-        <v>3063</v>
+        <v>956</v>
       </c>
       <c r="EB10" t="s">
         <v>172</v>
       </c>
-      <c r="EC10" t="s">
-        <v>956</v>
-      </c>
-      <c r="ED10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="11" spans="1:134">
+    </row>
+    <row r="11" spans="1:132">
       <c r="C11" t="s">
         <v>183</v>
       </c>
@@ -13639,26 +13542,26 @@
       <c r="DP11" t="s">
         <v>172</v>
       </c>
+      <c r="DW11" t="s">
+        <v>3041</v>
+      </c>
+      <c r="DX11" t="s">
+        <v>172</v>
+      </c>
       <c r="DY11" t="s">
-        <v>3051</v>
+        <v>3054</v>
       </c>
       <c r="DZ11" t="s">
         <v>172</v>
       </c>
       <c r="EA11" t="s">
-        <v>3064</v>
+        <v>957</v>
       </c>
       <c r="EB11" t="s">
         <v>172</v>
       </c>
-      <c r="EC11" t="s">
-        <v>957</v>
-      </c>
-      <c r="ED11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="12" spans="1:134">
+    </row>
+    <row r="12" spans="1:132">
       <c r="C12" t="s">
         <v>184</v>
       </c>
@@ -13839,26 +13742,26 @@
       <c r="DP12" t="s">
         <v>172</v>
       </c>
+      <c r="DW12" t="s">
+        <v>3042</v>
+      </c>
+      <c r="DX12" t="s">
+        <v>172</v>
+      </c>
       <c r="DY12" t="s">
-        <v>3052</v>
+        <v>3055</v>
       </c>
       <c r="DZ12" t="s">
         <v>172</v>
       </c>
       <c r="EA12" t="s">
-        <v>3065</v>
+        <v>958</v>
       </c>
       <c r="EB12" t="s">
         <v>172</v>
       </c>
-      <c r="EC12" t="s">
-        <v>958</v>
-      </c>
-      <c r="ED12" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="13" spans="1:134">
+    </row>
+    <row r="13" spans="1:132">
       <c r="C13" t="s">
         <v>185</v>
       </c>
@@ -14009,26 +13912,26 @@
       <c r="DL13" t="s">
         <v>172</v>
       </c>
+      <c r="DW13" t="s">
+        <v>3043</v>
+      </c>
+      <c r="DX13" t="s">
+        <v>172</v>
+      </c>
       <c r="DY13" t="s">
-        <v>3053</v>
+        <v>3056</v>
       </c>
       <c r="DZ13" t="s">
         <v>172</v>
       </c>
       <c r="EA13" t="s">
-        <v>3066</v>
+        <v>959</v>
       </c>
       <c r="EB13" t="s">
         <v>172</v>
       </c>
-      <c r="EC13" t="s">
-        <v>959</v>
-      </c>
-      <c r="ED13" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="14" spans="1:134">
+    </row>
+    <row r="14" spans="1:132">
       <c r="C14" t="s">
         <v>186</v>
       </c>
@@ -14173,26 +14076,26 @@
       <c r="DL14" t="s">
         <v>172</v>
       </c>
+      <c r="DW14" t="s">
+        <v>3044</v>
+      </c>
+      <c r="DX14" t="s">
+        <v>172</v>
+      </c>
       <c r="DY14" t="s">
-        <v>3054</v>
+        <v>3057</v>
       </c>
       <c r="DZ14" t="s">
         <v>172</v>
       </c>
       <c r="EA14" t="s">
-        <v>3067</v>
+        <v>960</v>
       </c>
       <c r="EB14" t="s">
         <v>172</v>
       </c>
-      <c r="EC14" t="s">
-        <v>960</v>
-      </c>
-      <c r="ED14" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="15" spans="1:134">
+    </row>
+    <row r="15" spans="1:132">
       <c r="C15" t="s">
         <v>187</v>
       </c>
@@ -14337,26 +14240,26 @@
       <c r="DL15" t="s">
         <v>172</v>
       </c>
+      <c r="DW15" t="s">
+        <v>3045</v>
+      </c>
+      <c r="DX15" t="s">
+        <v>172</v>
+      </c>
       <c r="DY15" t="s">
-        <v>3055</v>
+        <v>3058</v>
       </c>
       <c r="DZ15" t="s">
         <v>172</v>
       </c>
       <c r="EA15" t="s">
-        <v>3068</v>
+        <v>961</v>
       </c>
       <c r="EB15" t="s">
         <v>172</v>
       </c>
-      <c r="EC15" t="s">
-        <v>961</v>
-      </c>
-      <c r="ED15" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="16" spans="1:134">
+    </row>
+    <row r="16" spans="1:132">
       <c r="C16" t="s">
         <v>188</v>
       </c>
@@ -14501,26 +14404,26 @@
       <c r="DL16" t="s">
         <v>172</v>
       </c>
+      <c r="DW16" t="s">
+        <v>3046</v>
+      </c>
+      <c r="DX16" t="s">
+        <v>172</v>
+      </c>
       <c r="DY16" t="s">
-        <v>3056</v>
+        <v>3059</v>
       </c>
       <c r="DZ16" t="s">
         <v>172</v>
       </c>
       <c r="EA16" t="s">
-        <v>3069</v>
+        <v>962</v>
       </c>
       <c r="EB16" t="s">
         <v>172</v>
       </c>
-      <c r="EC16" t="s">
-        <v>962</v>
-      </c>
-      <c r="ED16" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="17" spans="7:134">
+    </row>
+    <row r="17" spans="7:132">
       <c r="G17" t="s">
         <v>208</v>
       </c>
@@ -14659,26 +14562,26 @@
       <c r="DL17" t="s">
         <v>172</v>
       </c>
+      <c r="DW17" t="s">
+        <v>952</v>
+      </c>
+      <c r="DX17" t="s">
+        <v>172</v>
+      </c>
       <c r="DY17" t="s">
-        <v>952</v>
+        <v>3060</v>
       </c>
       <c r="DZ17" t="s">
         <v>172</v>
       </c>
       <c r="EA17" t="s">
-        <v>3070</v>
+        <v>963</v>
       </c>
       <c r="EB17" t="s">
         <v>172</v>
       </c>
-      <c r="EC17" t="s">
-        <v>963</v>
-      </c>
-      <c r="ED17" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="18" spans="7:134">
+    </row>
+    <row r="18" spans="7:132">
       <c r="I18" t="s">
         <v>238</v>
       </c>
@@ -14799,20 +14702,20 @@
       <c r="DL18" t="s">
         <v>172</v>
       </c>
+      <c r="DY18" t="s">
+        <v>3061</v>
+      </c>
+      <c r="DZ18" t="s">
+        <v>172</v>
+      </c>
       <c r="EA18" t="s">
-        <v>3071</v>
+        <v>964</v>
       </c>
       <c r="EB18" t="s">
         <v>172</v>
       </c>
-      <c r="EC18" t="s">
-        <v>964</v>
-      </c>
-      <c r="ED18" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="19" spans="7:134">
+    </row>
+    <row r="19" spans="7:132">
       <c r="I19" t="s">
         <v>240</v>
       </c>
@@ -14927,20 +14830,20 @@
       <c r="DL19" t="s">
         <v>172</v>
       </c>
+      <c r="DY19" t="s">
+        <v>3062</v>
+      </c>
+      <c r="DZ19" t="s">
+        <v>172</v>
+      </c>
       <c r="EA19" t="s">
-        <v>3072</v>
+        <v>965</v>
       </c>
       <c r="EB19" t="s">
         <v>172</v>
       </c>
-      <c r="EC19" t="s">
-        <v>965</v>
-      </c>
-      <c r="ED19" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="20" spans="7:134">
+    </row>
+    <row r="20" spans="7:132">
       <c r="I20" t="s">
         <v>242</v>
       </c>
@@ -15055,20 +14958,20 @@
       <c r="DL20" t="s">
         <v>172</v>
       </c>
+      <c r="DY20" t="s">
+        <v>3063</v>
+      </c>
+      <c r="DZ20" t="s">
+        <v>172</v>
+      </c>
       <c r="EA20" t="s">
-        <v>3073</v>
+        <v>966</v>
       </c>
       <c r="EB20" t="s">
         <v>172</v>
       </c>
-      <c r="EC20" t="s">
-        <v>966</v>
-      </c>
-      <c r="ED20" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="21" spans="7:134">
+    </row>
+    <row r="21" spans="7:132">
       <c r="I21" t="s">
         <v>244</v>
       </c>
@@ -15159,20 +15062,20 @@
       <c r="DL21" t="s">
         <v>172</v>
       </c>
+      <c r="DY21" t="s">
+        <v>3064</v>
+      </c>
+      <c r="DZ21" t="s">
+        <v>172</v>
+      </c>
       <c r="EA21" t="s">
-        <v>3074</v>
+        <v>967</v>
       </c>
       <c r="EB21" t="s">
         <v>172</v>
       </c>
-      <c r="EC21" t="s">
-        <v>967</v>
-      </c>
-      <c r="ED21" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="22" spans="7:134">
+    </row>
+    <row r="22" spans="7:132">
       <c r="I22" t="s">
         <v>246</v>
       </c>
@@ -15263,20 +15166,20 @@
       <c r="DL22" t="s">
         <v>172</v>
       </c>
+      <c r="DY22" t="s">
+        <v>3065</v>
+      </c>
+      <c r="DZ22" t="s">
+        <v>172</v>
+      </c>
       <c r="EA22" t="s">
-        <v>3075</v>
+        <v>968</v>
       </c>
       <c r="EB22" t="s">
         <v>172</v>
       </c>
-      <c r="EC22" t="s">
-        <v>968</v>
-      </c>
-      <c r="ED22" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="23" spans="7:134">
+    </row>
+    <row r="23" spans="7:132">
       <c r="I23" t="s">
         <v>248</v>
       </c>
@@ -15367,20 +15270,20 @@
       <c r="DL23" t="s">
         <v>172</v>
       </c>
+      <c r="DY23" t="s">
+        <v>1871</v>
+      </c>
+      <c r="DZ23" t="s">
+        <v>172</v>
+      </c>
       <c r="EA23" t="s">
-        <v>1871</v>
+        <v>969</v>
       </c>
       <c r="EB23" t="s">
         <v>172</v>
       </c>
-      <c r="EC23" t="s">
-        <v>969</v>
-      </c>
-      <c r="ED23" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="24" spans="7:134">
+    </row>
+    <row r="24" spans="7:132">
       <c r="I24" t="s">
         <v>250</v>
       </c>
@@ -15459,20 +15362,20 @@
       <c r="DL24" t="s">
         <v>172</v>
       </c>
+      <c r="DY24" t="s">
+        <v>3066</v>
+      </c>
+      <c r="DZ24" t="s">
+        <v>172</v>
+      </c>
       <c r="EA24" t="s">
-        <v>3076</v>
+        <v>970</v>
       </c>
       <c r="EB24" t="s">
         <v>172</v>
       </c>
-      <c r="EC24" t="s">
-        <v>970</v>
-      </c>
-      <c r="ED24" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="25" spans="7:134">
+    </row>
+    <row r="25" spans="7:132">
       <c r="I25" t="s">
         <v>252</v>
       </c>
@@ -15551,20 +15454,20 @@
       <c r="DL25" t="s">
         <v>172</v>
       </c>
+      <c r="DY25" t="s">
+        <v>3067</v>
+      </c>
+      <c r="DZ25" t="s">
+        <v>172</v>
+      </c>
       <c r="EA25" t="s">
-        <v>3077</v>
+        <v>971</v>
       </c>
       <c r="EB25" t="s">
         <v>172</v>
       </c>
-      <c r="EC25" t="s">
-        <v>971</v>
-      </c>
-      <c r="ED25" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="26" spans="7:134">
+    </row>
+    <row r="26" spans="7:132">
       <c r="I26" t="s">
         <v>254</v>
       </c>
@@ -15637,20 +15540,20 @@
       <c r="DL26" t="s">
         <v>172</v>
       </c>
+      <c r="DY26" t="s">
+        <v>3068</v>
+      </c>
+      <c r="DZ26" t="s">
+        <v>172</v>
+      </c>
       <c r="EA26" t="s">
-        <v>3078</v>
+        <v>972</v>
       </c>
       <c r="EB26" t="s">
         <v>172</v>
       </c>
-      <c r="EC26" t="s">
-        <v>972</v>
-      </c>
-      <c r="ED26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="7:134">
+    </row>
+    <row r="27" spans="7:132">
       <c r="I27" t="s">
         <v>256</v>
       </c>
@@ -15723,20 +15626,20 @@
       <c r="DL27" t="s">
         <v>172</v>
       </c>
+      <c r="DY27" t="s">
+        <v>3069</v>
+      </c>
+      <c r="DZ27" t="s">
+        <v>172</v>
+      </c>
       <c r="EA27" t="s">
-        <v>3079</v>
+        <v>973</v>
       </c>
       <c r="EB27" t="s">
         <v>172</v>
       </c>
-      <c r="EC27" t="s">
-        <v>973</v>
-      </c>
-      <c r="ED27" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="28" spans="7:134">
+    </row>
+    <row r="28" spans="7:132">
       <c r="I28" t="s">
         <v>258</v>
       </c>
@@ -15809,14 +15712,14 @@
       <c r="DL28" t="s">
         <v>172</v>
       </c>
-      <c r="EC28" t="s">
+      <c r="EA28" t="s">
         <v>974</v>
       </c>
-      <c r="ED28" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="7:134">
+      <c r="EB28" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="7:132">
       <c r="I29" t="s">
         <v>260</v>
       </c>
@@ -15889,14 +15792,14 @@
       <c r="DL29" t="s">
         <v>172</v>
       </c>
-      <c r="EC29" t="s">
+      <c r="EA29" t="s">
         <v>975</v>
       </c>
-      <c r="ED29" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="30" spans="7:134">
+      <c r="EB29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="7:132">
       <c r="I30" t="s">
         <v>262</v>
       </c>
@@ -15969,14 +15872,14 @@
       <c r="DL30" t="s">
         <v>172</v>
       </c>
-      <c r="EC30" t="s">
+      <c r="EA30" t="s">
         <v>976</v>
       </c>
-      <c r="ED30" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="31" spans="7:134">
+      <c r="EB30" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="31" spans="7:132">
       <c r="I31" t="s">
         <v>264</v>
       </c>
@@ -16049,14 +15952,14 @@
       <c r="DL31" t="s">
         <v>172</v>
       </c>
-      <c r="EC31" t="s">
+      <c r="EA31" t="s">
         <v>977</v>
       </c>
-      <c r="ED31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="32" spans="7:134">
+      <c r="EB31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="7:132">
       <c r="I32" t="s">
         <v>266</v>
       </c>
@@ -16129,14 +16032,14 @@
       <c r="DL32" t="s">
         <v>172</v>
       </c>
-      <c r="EC32" t="s">
+      <c r="EA32" t="s">
         <v>978</v>
       </c>
-      <c r="ED32" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="33" spans="9:134">
+      <c r="EB32" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="33" spans="9:132">
       <c r="I33" t="s">
         <v>268</v>
       </c>
@@ -16209,14 +16112,14 @@
       <c r="DL33" t="s">
         <v>172</v>
       </c>
-      <c r="EC33" t="s">
+      <c r="EA33" t="s">
         <v>979</v>
       </c>
-      <c r="ED33" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="34" spans="9:134">
+      <c r="EB33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="9:132">
       <c r="I34" t="s">
         <v>270</v>
       </c>
@@ -16289,14 +16192,14 @@
       <c r="DL34" t="s">
         <v>172</v>
       </c>
-      <c r="EC34" t="s">
+      <c r="EA34" t="s">
         <v>980</v>
       </c>
-      <c r="ED34" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="35" spans="9:134">
+      <c r="EB34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="9:132">
       <c r="I35" t="s">
         <v>272</v>
       </c>
@@ -16369,14 +16272,14 @@
       <c r="DL35" t="s">
         <v>172</v>
       </c>
-      <c r="EC35" t="s">
+      <c r="EA35" t="s">
         <v>981</v>
       </c>
-      <c r="ED35" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="36" spans="9:134">
+      <c r="EB35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="9:132">
       <c r="I36" t="s">
         <v>274</v>
       </c>
@@ -16449,14 +16352,14 @@
       <c r="DL36" t="s">
         <v>172</v>
       </c>
-      <c r="EC36" t="s">
+      <c r="EA36" t="s">
         <v>982</v>
       </c>
-      <c r="ED36" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="37" spans="9:134">
+      <c r="EB36" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="37" spans="9:132">
       <c r="I37" t="s">
         <v>276</v>
       </c>
@@ -16529,14 +16432,14 @@
       <c r="DL37" t="s">
         <v>172</v>
       </c>
-      <c r="EC37" t="s">
+      <c r="EA37" t="s">
         <v>983</v>
       </c>
-      <c r="ED37" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="38" spans="9:134">
+      <c r="EB37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="9:132">
       <c r="I38" t="s">
         <v>278</v>
       </c>
@@ -16609,14 +16512,14 @@
       <c r="DL38" t="s">
         <v>172</v>
       </c>
-      <c r="EC38" t="s">
+      <c r="EA38" t="s">
         <v>984</v>
       </c>
-      <c r="ED38" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="39" spans="9:134">
+      <c r="EB38" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="9:132">
       <c r="I39" t="s">
         <v>280</v>
       </c>
@@ -16689,14 +16592,14 @@
       <c r="DL39" t="s">
         <v>172</v>
       </c>
-      <c r="EC39" t="s">
+      <c r="EA39" t="s">
         <v>985</v>
       </c>
-      <c r="ED39" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="9:134">
+      <c r="EB39" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="40" spans="9:132">
       <c r="I40" t="s">
         <v>282</v>
       </c>
@@ -16769,14 +16672,14 @@
       <c r="DL40" t="s">
         <v>172</v>
       </c>
-      <c r="EC40" t="s">
+      <c r="EA40" t="s">
         <v>986</v>
       </c>
-      <c r="ED40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="9:134">
+      <c r="EB40" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="41" spans="9:132">
       <c r="I41" t="s">
         <v>284</v>
       </c>
@@ -16849,14 +16752,14 @@
       <c r="DL41" t="s">
         <v>172</v>
       </c>
-      <c r="EC41" t="s">
+      <c r="EA41" t="s">
         <v>987</v>
       </c>
-      <c r="ED41" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="42" spans="9:134">
+      <c r="EB41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="9:132">
       <c r="I42" t="s">
         <v>286</v>
       </c>
@@ -16929,14 +16832,14 @@
       <c r="DL42" t="s">
         <v>172</v>
       </c>
-      <c r="EC42" t="s">
+      <c r="EA42" t="s">
         <v>988</v>
       </c>
-      <c r="ED42" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="43" spans="9:134">
+      <c r="EB42" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="9:132">
       <c r="I43" t="s">
         <v>288</v>
       </c>
@@ -17009,14 +16912,14 @@
       <c r="DL43" t="s">
         <v>172</v>
       </c>
-      <c r="EC43" t="s">
+      <c r="EA43" t="s">
         <v>989</v>
       </c>
-      <c r="ED43" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" spans="9:134">
+      <c r="EB43" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="44" spans="9:132">
       <c r="I44" t="s">
         <v>290</v>
       </c>
@@ -17089,14 +16992,14 @@
       <c r="DL44" t="s">
         <v>172</v>
       </c>
-      <c r="EC44" t="s">
+      <c r="EA44" t="s">
         <v>990</v>
       </c>
-      <c r="ED44" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="9:134">
+      <c r="EB44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="9:132">
       <c r="I45" t="s">
         <v>292</v>
       </c>
@@ -17169,14 +17072,14 @@
       <c r="DL45" t="s">
         <v>172</v>
       </c>
-      <c r="EC45" t="s">
+      <c r="EA45" t="s">
         <v>991</v>
       </c>
-      <c r="ED45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="9:134">
+      <c r="EB45" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="46" spans="9:132">
       <c r="I46" t="s">
         <v>294</v>
       </c>
@@ -17249,14 +17152,14 @@
       <c r="DL46" t="s">
         <v>172</v>
       </c>
-      <c r="EC46" t="s">
+      <c r="EA46" t="s">
         <v>992</v>
       </c>
-      <c r="ED46" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="47" spans="9:134">
+      <c r="EB46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="9:132">
       <c r="I47" t="s">
         <v>296</v>
       </c>
@@ -17329,14 +17232,14 @@
       <c r="DL47" t="s">
         <v>172</v>
       </c>
-      <c r="EC47" t="s">
+      <c r="EA47" t="s">
         <v>993</v>
       </c>
-      <c r="ED47" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="48" spans="9:134">
+      <c r="EB47" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="48" spans="9:132">
       <c r="I48" t="s">
         <v>298</v>
       </c>
@@ -17409,14 +17312,14 @@
       <c r="DL48" t="s">
         <v>172</v>
       </c>
-      <c r="EC48" t="s">
+      <c r="EA48" t="s">
         <v>994</v>
       </c>
-      <c r="ED48" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="49" spans="9:134">
+      <c r="EB48" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="49" spans="9:132">
       <c r="I49" t="s">
         <v>300</v>
       </c>
@@ -17489,14 +17392,14 @@
       <c r="DL49" t="s">
         <v>172</v>
       </c>
-      <c r="EC49" t="s">
+      <c r="EA49" t="s">
         <v>995</v>
       </c>
-      <c r="ED49" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="50" spans="9:134">
+      <c r="EB49" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="50" spans="9:132">
       <c r="I50" t="s">
         <v>302</v>
       </c>
@@ -17569,14 +17472,14 @@
       <c r="DL50" t="s">
         <v>172</v>
       </c>
-      <c r="EC50" t="s">
+      <c r="EA50" t="s">
         <v>996</v>
       </c>
-      <c r="ED50" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="51" spans="9:134">
+      <c r="EB50" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="51" spans="9:132">
       <c r="I51" t="s">
         <v>304</v>
       </c>
@@ -17649,14 +17552,14 @@
       <c r="DL51" t="s">
         <v>172</v>
       </c>
-      <c r="EC51" t="s">
+      <c r="EA51" t="s">
         <v>997</v>
       </c>
-      <c r="ED51" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="9:134">
+      <c r="EB51" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="9:132">
       <c r="I52" t="s">
         <v>306</v>
       </c>
@@ -17723,14 +17626,14 @@
       <c r="DL52" t="s">
         <v>172</v>
       </c>
-      <c r="EC52" t="s">
+      <c r="EA52" t="s">
         <v>998</v>
       </c>
-      <c r="ED52" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="53" spans="9:134">
+      <c r="EB52" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="9:132">
       <c r="I53" t="s">
         <v>308</v>
       </c>
@@ -17797,14 +17700,14 @@
       <c r="DL53" t="s">
         <v>172</v>
       </c>
-      <c r="EC53" t="s">
+      <c r="EA53" t="s">
         <v>999</v>
       </c>
-      <c r="ED53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="54" spans="9:134">
+      <c r="EB53" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="54" spans="9:132">
       <c r="I54" t="s">
         <v>310</v>
       </c>
@@ -17871,14 +17774,14 @@
       <c r="DL54" t="s">
         <v>172</v>
       </c>
-      <c r="EC54" t="s">
+      <c r="EA54" t="s">
         <v>1000</v>
       </c>
-      <c r="ED54" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="55" spans="9:134">
+      <c r="EB54" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="55" spans="9:132">
       <c r="I55" t="s">
         <v>312</v>
       </c>
@@ -17945,14 +17848,14 @@
       <c r="DL55" t="s">
         <v>172</v>
       </c>
-      <c r="EC55" t="s">
+      <c r="EA55" t="s">
         <v>1001</v>
       </c>
-      <c r="ED55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="9:134">
+      <c r="EB55" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="56" spans="9:132">
       <c r="I56" t="s">
         <v>314</v>
       </c>
@@ -18019,14 +17922,14 @@
       <c r="DL56" t="s">
         <v>172</v>
       </c>
-      <c r="EC56" t="s">
+      <c r="EA56" t="s">
         <v>1002</v>
       </c>
-      <c r="ED56" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="57" spans="9:134">
+      <c r="EB56" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="57" spans="9:132">
       <c r="I57" t="s">
         <v>316</v>
       </c>
@@ -18093,14 +17996,14 @@
       <c r="DL57" t="s">
         <v>172</v>
       </c>
-      <c r="EC57" t="s">
+      <c r="EA57" t="s">
         <v>1003</v>
       </c>
-      <c r="ED57" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="58" spans="9:134">
+      <c r="EB57" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="58" spans="9:132">
       <c r="I58" t="s">
         <v>318</v>
       </c>
@@ -18167,14 +18070,14 @@
       <c r="DL58" t="s">
         <v>172</v>
       </c>
-      <c r="EC58" t="s">
+      <c r="EA58" t="s">
         <v>1004</v>
       </c>
-      <c r="ED58" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="59" spans="9:134">
+      <c r="EB58" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="59" spans="9:132">
       <c r="I59" t="s">
         <v>320</v>
       </c>
@@ -18241,14 +18144,14 @@
       <c r="DL59" t="s">
         <v>172</v>
       </c>
-      <c r="EC59" t="s">
+      <c r="EA59" t="s">
         <v>1005</v>
       </c>
-      <c r="ED59" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="60" spans="9:134">
+      <c r="EB59" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="60" spans="9:132">
       <c r="I60" t="s">
         <v>322</v>
       </c>
@@ -18315,14 +18218,14 @@
       <c r="DL60" t="s">
         <v>172</v>
       </c>
-      <c r="EC60" t="s">
+      <c r="EA60" t="s">
         <v>1006</v>
       </c>
-      <c r="ED60" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="61" spans="9:134">
+      <c r="EB60" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="61" spans="9:132">
       <c r="I61" t="s">
         <v>324</v>
       </c>
@@ -18372,7 +18275,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="62" spans="9:134">
+    <row r="62" spans="9:132">
       <c r="I62" t="s">
         <v>326</v>
       </c>
@@ -18422,7 +18325,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="63" spans="9:134">
+    <row r="63" spans="9:132">
       <c r="I63" t="s">
         <v>328</v>
       </c>
@@ -18472,7 +18375,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="64" spans="9:134">
+    <row r="64" spans="9:132">
       <c r="I64" t="s">
         <v>330</v>
       </c>
@@ -33557,7 +33460,7 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="72">
+  <mergeCells count="70">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
@@ -33624,15 +33527,13 @@
     <mergeCell ref="DS2:DT2"/>
     <mergeCell ref="BQ1:DT1"/>
     <mergeCell ref="DU2:DV2"/>
-    <mergeCell ref="DU1:DV1"/>
     <mergeCell ref="DW2:DX2"/>
     <mergeCell ref="DY2:DZ2"/>
     <mergeCell ref="EA2:EB2"/>
-    <mergeCell ref="EC2:ED2"/>
-    <mergeCell ref="DW1:ED1"/>
+    <mergeCell ref="DU1:EB1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="67">
+  <tableParts count="66">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
@@ -33699,7 +33600,6 @@
     <tablePart r:id="rId64"/>
     <tablePart r:id="rId65"/>
     <tablePart r:id="rId66"/>
-    <tablePart r:id="rId67"/>
   </tableParts>
 </worksheet>
 </file>
@@ -38917,127 +38817,6 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46.7109375" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="32.7109375" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="50.7109375" style="2" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" hidden="1">
-      <c r="A1" s="3" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1568</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1569</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2989</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2991</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>2993</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2995</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1">
-      <c r="A2" s="4" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="1" t="s">
-        <v>2997</v>
-      </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" hidden="1">
-      <c r="B3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>1008</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>2990</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>2992</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>2994</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>2996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="3" t="s">
-        <v>1007</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>1568</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>1569</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>2989</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>2991</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>2993</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>2995</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-  </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5:C1000001">
-      <formula1>'Codelijsten'!$DU$4:$DU$10</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:F1000001">
-      <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G1000001">
-      <formula1>1</formula1>
-    </dataValidation>
-  </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="C4" location="'Codelijsten'!$DU$2" display="filter-filtertype"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BC6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -39106,58 +38885,58 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>2989</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2990</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2991</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2992</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2993</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>2994</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>2995</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>2996</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>2997</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>2999</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>3000</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>3001</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3002</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>3003</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>3004</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>3005</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>3006</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>3007</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>3009</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>3010</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>3011</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>3012</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>3013</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>3014</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>3015</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>3016</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>3017</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>4</v>
@@ -39166,58 +38945,58 @@
         <v>6</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>3019</v>
+        <v>3009</v>
       </c>
       <c r="W1" s="1" t="s">
+        <v>3010</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>3012</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>3013</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>3016</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="AF1" s="1" t="s">
         <v>3020</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>3021</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>3022</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>3023</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>3024</v>
-      </c>
-      <c r="AB1" s="1" t="s">
-        <v>3025</v>
-      </c>
-      <c r="AC1" s="1" t="s">
-        <v>3026</v>
-      </c>
-      <c r="AD1" s="1" t="s">
-        <v>3027</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>3028</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>3030</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>3031</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>3032</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>3034</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>3037</v>
+        <v>3027</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>3039</v>
+        <v>3029</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>3041</v>
+        <v>3031</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>152</v>
@@ -39273,7 +39052,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3008</v>
+        <v>2998</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -39284,7 +39063,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>3018</v>
+        <v>3008</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -39299,10 +39078,10 @@
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
+        <v>3009</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>3019</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>3029</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -39313,20 +39092,20 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1" t="s">
-        <v>3030</v>
+        <v>3020</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>3031</v>
+        <v>3021</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>3036</v>
+        <v>3026</v>
       </c>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>3043</v>
+        <v>3033</v>
       </c>
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
@@ -39400,19 +39179,19 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AH3" s="4" t="s">
-        <v>3033</v>
+        <v>3023</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>3035</v>
+        <v>3025</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>3038</v>
+        <v>3028</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>3040</v>
+        <v>3030</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>3042</v>
+        <v>3032</v>
       </c>
       <c r="AO3" s="4" t="s">
         <v>143</v>
@@ -39580,58 +39359,58 @@
         <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>2998</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2990</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2991</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2992</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2993</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>2994</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>2995</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>2996</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>2997</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>3008</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>3000</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="M6" s="1" t="s">
         <v>3001</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>3002</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="O6" s="1" t="s">
         <v>3003</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>3004</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>3005</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="R6" s="1" t="s">
         <v>3006</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>3007</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>3018</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>3010</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>3011</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>3012</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>3013</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>3014</v>
-      </c>
-      <c r="Q6" s="1" t="s">
-        <v>3015</v>
-      </c>
-      <c r="R6" s="1" t="s">
-        <v>3016</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>3017</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>4</v>
@@ -39640,58 +39419,58 @@
         <v>6</v>
       </c>
       <c r="V6" s="1" t="s">
+        <v>3009</v>
+      </c>
+      <c r="W6" s="1" t="s">
         <v>3019</v>
       </c>
-      <c r="W6" s="1" t="s">
-        <v>3029</v>
-      </c>
       <c r="X6" s="1" t="s">
+        <v>3011</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>3012</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>3013</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>3014</v>
+      </c>
+      <c r="AB6" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="AC6" s="1" t="s">
+        <v>3016</v>
+      </c>
+      <c r="AD6" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="AE6" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="AF6" s="1" t="s">
+        <v>3020</v>
+      </c>
+      <c r="AG6" s="1" t="s">
         <v>3021</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="AH6" s="1" t="s">
         <v>3022</v>
       </c>
-      <c r="Z6" s="1" t="s">
-        <v>3023</v>
-      </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AI6" s="1" t="s">
         <v>3024</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>3025</v>
-      </c>
-      <c r="AC6" s="1" t="s">
-        <v>3026</v>
-      </c>
-      <c r="AD6" s="1" t="s">
-        <v>3027</v>
-      </c>
-      <c r="AE6" s="1" t="s">
-        <v>3028</v>
-      </c>
-      <c r="AF6" s="1" t="s">
-        <v>3030</v>
-      </c>
-      <c r="AG6" s="1" t="s">
-        <v>3031</v>
-      </c>
-      <c r="AH6" s="1" t="s">
-        <v>3032</v>
-      </c>
-      <c r="AI6" s="1" t="s">
-        <v>3034</v>
       </c>
       <c r="AJ6" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>3037</v>
+        <v>3027</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>3039</v>
+        <v>3029</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>3041</v>
+        <v>3031</v>
       </c>
       <c r="AN6" s="1" t="s">
         <v>152</v>
@@ -39773,13 +39552,13 @@
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7:AJ1000001">
-      <formula1>'Codelijsten'!$DW$4:$DW$8</formula1>
+      <formula1>'Codelijsten'!$DU$4:$DU$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL7:AL1000001">
-      <formula1>'Codelijsten'!$DY$4:$DY$17</formula1>
+      <formula1>'Codelijsten'!$DW$4:$DW$17</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM7:AM1000001">
-      <formula1>'Codelijsten'!$EA$4:$EA$27</formula1>
+      <formula1>'Codelijsten'!$DY$4:$DY$27</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU7:AU1000001">
       <formula1>1</formula1>
@@ -39788,14 +39567,14 @@
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB7:BB1000001">
-      <formula1>'Codelijsten'!$EC$4:$EC$60</formula1>
+      <formula1>'Codelijsten'!$EA$4:$EA$60</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="AJ6" location="'Codelijsten'!$DW$2" display="status"/>
-    <hyperlink ref="AL6" location="'Codelijsten'!$DY$2" display="kwaliteit-origine"/>
-    <hyperlink ref="AM6" location="'Codelijsten'!$EA$2" display="kwaliteit-aard"/>
-    <hyperlink ref="BB6" location="'Codelijsten'!$EC$2" display="bijlage-bijlage_type"/>
+    <hyperlink ref="AJ6" location="'Codelijsten'!$DU$2" display="status"/>
+    <hyperlink ref="AL6" location="'Codelijsten'!$DW$2" display="kwaliteit-origine"/>
+    <hyperlink ref="AM6" location="'Codelijsten'!$DY$2" display="kwaliteit-aard"/>
+    <hyperlink ref="BB6" location="'Codelijsten'!$EA$2" display="bijlage-bijlage_type"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added testing of the main converting functionality
</commit_message>
<xml_diff>
--- a/data/grondwater_template.xlsx
+++ b/data/grondwater_template.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8473" uniqueCount="3070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8489" uniqueCount="3074">
   <si>
     <t>identificatie</t>
   </si>
@@ -8339,6 +8339,15 @@
     <t>PFHxSbranched</t>
   </si>
   <si>
+    <t>Bepaling kleihoudendheid in fractie 0-0.125 mm</t>
+  </si>
+  <si>
+    <t>Bepaling kleihoudendheid in fractie 0-2 mm</t>
+  </si>
+  <si>
+    <t>Grondsoort RIG</t>
+  </si>
+  <si>
     <t>resultaattijd</t>
   </si>
   <si>
@@ -8400,6 +8409,9 @@
   </si>
   <si>
     <t>g MB/100g droog monster</t>
+  </si>
+  <si>
+    <t>g MB/1000g droog monster</t>
   </si>
   <si>
     <t>°C</t>
@@ -9802,7 +9814,7 @@
 </file>
 
 <file path=xl/tables/table52.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="CY3:CZ918" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="52" name="Table52" displayName="Table52" ref="CY3:CZ921" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -9812,7 +9824,7 @@
 </file>
 
 <file path=xl/tables/table53.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="53" name="Table53" displayName="Table53" ref="DA3:DB66" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="53" name="Table53" displayName="Table53" ref="DA3:DB67" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -9852,7 +9864,7 @@
 </file>
 
 <file path=xl/tables/table57.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="Table57" displayName="Table57" ref="DI3:DJ918" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="57" name="Table57" displayName="Table57" ref="DI3:DJ921" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -9862,7 +9874,7 @@
 </file>
 
 <file path=xl/tables/table58.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="Table58" displayName="Table58" ref="DK3:DL66" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="58" name="Table58" displayName="Table58" ref="DK3:DL67" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Code"/>
     <tableColumn id="2" name="Beschrijving"/>
@@ -10276,7 +10288,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:EB918"/>
+  <dimension ref="A1:EB921"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -10359,7 +10371,7 @@
       <c r="BO1" s="1"/>
       <c r="BP1" s="1"/>
       <c r="BQ1" s="1" t="s">
-        <v>2988</v>
+        <v>2992</v>
       </c>
       <c r="BR1" s="1"/>
       <c r="BS1" s="1"/>
@@ -10681,11 +10693,11 @@
       </c>
       <c r="DV2" s="1"/>
       <c r="DW2" s="1" t="s">
-        <v>3029</v>
+        <v>3033</v>
       </c>
       <c r="DX2" s="1"/>
       <c r="DY2" s="1" t="s">
-        <v>3031</v>
+        <v>3035</v>
       </c>
       <c r="DZ2" s="1"/>
       <c r="EA2" s="1" t="s">
@@ -11405,13 +11417,13 @@
         <v>172</v>
       </c>
       <c r="DA4" t="s">
-        <v>2779</v>
+        <v>2782</v>
       </c>
       <c r="DB4" t="s">
         <v>172</v>
       </c>
       <c r="DC4" t="s">
-        <v>2839</v>
+        <v>2843</v>
       </c>
       <c r="DD4" t="s">
         <v>172</v>
@@ -11435,7 +11447,7 @@
         <v>172</v>
       </c>
       <c r="DK4" t="s">
-        <v>2779</v>
+        <v>2782</v>
       </c>
       <c r="DL4" t="s">
         <v>172</v>
@@ -11459,7 +11471,7 @@
         <v>172</v>
       </c>
       <c r="DS4" t="s">
-        <v>2985</v>
+        <v>2989</v>
       </c>
       <c r="DT4" t="s">
         <v>172</v>
@@ -11471,13 +11483,13 @@
         <v>172</v>
       </c>
       <c r="DW4" t="s">
-        <v>3034</v>
+        <v>3038</v>
       </c>
       <c r="DX4" t="s">
         <v>172</v>
       </c>
       <c r="DY4" t="s">
-        <v>3047</v>
+        <v>3051</v>
       </c>
       <c r="DZ4" t="s">
         <v>172</v>
@@ -11803,13 +11815,13 @@
         <v>172</v>
       </c>
       <c r="DA5" t="s">
-        <v>2780</v>
+        <v>2783</v>
       </c>
       <c r="DB5" t="s">
         <v>172</v>
       </c>
       <c r="DC5" t="s">
-        <v>2840</v>
+        <v>2844</v>
       </c>
       <c r="DD5" t="s">
         <v>172</v>
@@ -11821,7 +11833,7 @@
         <v>172</v>
       </c>
       <c r="DG5" t="s">
-        <v>2984</v>
+        <v>2988</v>
       </c>
       <c r="DH5" t="s">
         <v>172</v>
@@ -11833,7 +11845,7 @@
         <v>172</v>
       </c>
       <c r="DK5" t="s">
-        <v>2780</v>
+        <v>2783</v>
       </c>
       <c r="DL5" t="s">
         <v>172</v>
@@ -11857,7 +11869,7 @@
         <v>172</v>
       </c>
       <c r="DS5" t="s">
-        <v>2986</v>
+        <v>2990</v>
       </c>
       <c r="DT5" t="s">
         <v>172</v>
@@ -11869,13 +11881,13 @@
         <v>172</v>
       </c>
       <c r="DW5" t="s">
-        <v>3035</v>
+        <v>3039</v>
       </c>
       <c r="DX5" t="s">
         <v>172</v>
       </c>
       <c r="DY5" t="s">
-        <v>3048</v>
+        <v>3052</v>
       </c>
       <c r="DZ5" t="s">
         <v>172</v>
@@ -12195,13 +12207,13 @@
         <v>172</v>
       </c>
       <c r="DA6" t="s">
-        <v>2781</v>
+        <v>2784</v>
       </c>
       <c r="DB6" t="s">
         <v>172</v>
       </c>
       <c r="DC6" t="s">
-        <v>2841</v>
+        <v>2845</v>
       </c>
       <c r="DD6" t="s">
         <v>172</v>
@@ -12219,7 +12231,7 @@
         <v>172</v>
       </c>
       <c r="DK6" t="s">
-        <v>2781</v>
+        <v>2784</v>
       </c>
       <c r="DL6" t="s">
         <v>172</v>
@@ -12243,7 +12255,7 @@
         <v>172</v>
       </c>
       <c r="DS6" t="s">
-        <v>2987</v>
+        <v>2991</v>
       </c>
       <c r="DT6" t="s">
         <v>172</v>
@@ -12255,13 +12267,13 @@
         <v>172</v>
       </c>
       <c r="DW6" t="s">
-        <v>3036</v>
+        <v>3040</v>
       </c>
       <c r="DX6" t="s">
         <v>172</v>
       </c>
       <c r="DY6" t="s">
-        <v>3049</v>
+        <v>3053</v>
       </c>
       <c r="DZ6" t="s">
         <v>172</v>
@@ -12521,13 +12533,13 @@
         <v>172</v>
       </c>
       <c r="DA7" t="s">
-        <v>2782</v>
+        <v>2785</v>
       </c>
       <c r="DB7" t="s">
         <v>172</v>
       </c>
       <c r="DC7" t="s">
-        <v>2842</v>
+        <v>2846</v>
       </c>
       <c r="DD7" t="s">
         <v>172</v>
@@ -12539,7 +12551,7 @@
         <v>172</v>
       </c>
       <c r="DK7" t="s">
-        <v>2782</v>
+        <v>2785</v>
       </c>
       <c r="DL7" t="s">
         <v>172</v>
@@ -12557,13 +12569,13 @@
         <v>172</v>
       </c>
       <c r="DW7" t="s">
-        <v>3037</v>
+        <v>3041</v>
       </c>
       <c r="DX7" t="s">
         <v>172</v>
       </c>
       <c r="DY7" t="s">
-        <v>3050</v>
+        <v>3054</v>
       </c>
       <c r="DZ7" t="s">
         <v>172</v>
@@ -12805,13 +12817,13 @@
         <v>172</v>
       </c>
       <c r="DA8" t="s">
-        <v>2783</v>
+        <v>2786</v>
       </c>
       <c r="DB8" t="s">
         <v>172</v>
       </c>
       <c r="DC8" t="s">
-        <v>2843</v>
+        <v>2847</v>
       </c>
       <c r="DD8" t="s">
         <v>172</v>
@@ -12823,7 +12835,7 @@
         <v>172</v>
       </c>
       <c r="DK8" t="s">
-        <v>2783</v>
+        <v>2786</v>
       </c>
       <c r="DL8" t="s">
         <v>172</v>
@@ -12841,13 +12853,13 @@
         <v>172</v>
       </c>
       <c r="DW8" t="s">
-        <v>3038</v>
+        <v>3042</v>
       </c>
       <c r="DX8" t="s">
         <v>172</v>
       </c>
       <c r="DY8" t="s">
-        <v>3051</v>
+        <v>3055</v>
       </c>
       <c r="DZ8" t="s">
         <v>172</v>
@@ -13059,13 +13071,13 @@
         <v>172</v>
       </c>
       <c r="DA9" t="s">
-        <v>2784</v>
+        <v>2787</v>
       </c>
       <c r="DB9" t="s">
         <v>172</v>
       </c>
       <c r="DC9" t="s">
-        <v>2844</v>
+        <v>2848</v>
       </c>
       <c r="DD9" t="s">
         <v>172</v>
@@ -13077,7 +13089,7 @@
         <v>172</v>
       </c>
       <c r="DK9" t="s">
-        <v>2784</v>
+        <v>2787</v>
       </c>
       <c r="DL9" t="s">
         <v>172</v>
@@ -13089,13 +13101,13 @@
         <v>172</v>
       </c>
       <c r="DW9" t="s">
-        <v>3039</v>
+        <v>3043</v>
       </c>
       <c r="DX9" t="s">
         <v>172</v>
       </c>
       <c r="DY9" t="s">
-        <v>3052</v>
+        <v>3056</v>
       </c>
       <c r="DZ9" t="s">
         <v>172</v>
@@ -13295,13 +13307,13 @@
         <v>172</v>
       </c>
       <c r="DA10" t="s">
-        <v>2785</v>
+        <v>2788</v>
       </c>
       <c r="DB10" t="s">
         <v>172</v>
       </c>
       <c r="DC10" t="s">
-        <v>2845</v>
+        <v>2849</v>
       </c>
       <c r="DD10" t="s">
         <v>172</v>
@@ -13313,7 +13325,7 @@
         <v>172</v>
       </c>
       <c r="DK10" t="s">
-        <v>2785</v>
+        <v>2788</v>
       </c>
       <c r="DL10" t="s">
         <v>172</v>
@@ -13325,13 +13337,13 @@
         <v>172</v>
       </c>
       <c r="DW10" t="s">
-        <v>3040</v>
+        <v>3044</v>
       </c>
       <c r="DX10" t="s">
         <v>172</v>
       </c>
       <c r="DY10" t="s">
-        <v>3053</v>
+        <v>3057</v>
       </c>
       <c r="DZ10" t="s">
         <v>172</v>
@@ -13513,13 +13525,13 @@
         <v>172</v>
       </c>
       <c r="DA11" t="s">
-        <v>2786</v>
+        <v>2789</v>
       </c>
       <c r="DB11" t="s">
         <v>172</v>
       </c>
       <c r="DC11" t="s">
-        <v>2846</v>
+        <v>2850</v>
       </c>
       <c r="DD11" t="s">
         <v>172</v>
@@ -13531,7 +13543,7 @@
         <v>172</v>
       </c>
       <c r="DK11" t="s">
-        <v>2786</v>
+        <v>2789</v>
       </c>
       <c r="DL11" t="s">
         <v>172</v>
@@ -13543,13 +13555,13 @@
         <v>172</v>
       </c>
       <c r="DW11" t="s">
-        <v>3041</v>
+        <v>3045</v>
       </c>
       <c r="DX11" t="s">
         <v>172</v>
       </c>
       <c r="DY11" t="s">
-        <v>3054</v>
+        <v>3058</v>
       </c>
       <c r="DZ11" t="s">
         <v>172</v>
@@ -13713,13 +13725,13 @@
         <v>172</v>
       </c>
       <c r="DA12" t="s">
-        <v>2787</v>
+        <v>2790</v>
       </c>
       <c r="DB12" t="s">
         <v>172</v>
       </c>
       <c r="DC12" t="s">
-        <v>2847</v>
+        <v>2851</v>
       </c>
       <c r="DD12" t="s">
         <v>172</v>
@@ -13731,7 +13743,7 @@
         <v>172</v>
       </c>
       <c r="DK12" t="s">
-        <v>2787</v>
+        <v>2790</v>
       </c>
       <c r="DL12" t="s">
         <v>172</v>
@@ -13743,13 +13755,13 @@
         <v>172</v>
       </c>
       <c r="DW12" t="s">
-        <v>3042</v>
+        <v>3046</v>
       </c>
       <c r="DX12" t="s">
         <v>172</v>
       </c>
       <c r="DY12" t="s">
-        <v>3055</v>
+        <v>3059</v>
       </c>
       <c r="DZ12" t="s">
         <v>172</v>
@@ -13889,13 +13901,13 @@
         <v>172</v>
       </c>
       <c r="DA13" t="s">
-        <v>2788</v>
+        <v>2791</v>
       </c>
       <c r="DB13" t="s">
         <v>172</v>
       </c>
       <c r="DC13" t="s">
-        <v>2848</v>
+        <v>2852</v>
       </c>
       <c r="DD13" t="s">
         <v>172</v>
@@ -13907,19 +13919,19 @@
         <v>172</v>
       </c>
       <c r="DK13" t="s">
-        <v>2788</v>
+        <v>2791</v>
       </c>
       <c r="DL13" t="s">
         <v>172</v>
       </c>
       <c r="DW13" t="s">
-        <v>3043</v>
+        <v>3047</v>
       </c>
       <c r="DX13" t="s">
         <v>172</v>
       </c>
       <c r="DY13" t="s">
-        <v>3056</v>
+        <v>3060</v>
       </c>
       <c r="DZ13" t="s">
         <v>172</v>
@@ -14053,13 +14065,13 @@
         <v>172</v>
       </c>
       <c r="DA14" t="s">
-        <v>2789</v>
+        <v>2792</v>
       </c>
       <c r="DB14" t="s">
         <v>172</v>
       </c>
       <c r="DC14" t="s">
-        <v>2849</v>
+        <v>2853</v>
       </c>
       <c r="DD14" t="s">
         <v>172</v>
@@ -14071,19 +14083,19 @@
         <v>172</v>
       </c>
       <c r="DK14" t="s">
-        <v>2789</v>
+        <v>2792</v>
       </c>
       <c r="DL14" t="s">
         <v>172</v>
       </c>
       <c r="DW14" t="s">
-        <v>3044</v>
+        <v>3048</v>
       </c>
       <c r="DX14" t="s">
         <v>172</v>
       </c>
       <c r="DY14" t="s">
-        <v>3057</v>
+        <v>3061</v>
       </c>
       <c r="DZ14" t="s">
         <v>172</v>
@@ -14217,13 +14229,13 @@
         <v>172</v>
       </c>
       <c r="DA15" t="s">
-        <v>2790</v>
+        <v>2793</v>
       </c>
       <c r="DB15" t="s">
         <v>172</v>
       </c>
       <c r="DC15" t="s">
-        <v>2850</v>
+        <v>2854</v>
       </c>
       <c r="DD15" t="s">
         <v>172</v>
@@ -14235,19 +14247,19 @@
         <v>172</v>
       </c>
       <c r="DK15" t="s">
-        <v>2790</v>
+        <v>2793</v>
       </c>
       <c r="DL15" t="s">
         <v>172</v>
       </c>
       <c r="DW15" t="s">
-        <v>3045</v>
+        <v>3049</v>
       </c>
       <c r="DX15" t="s">
         <v>172</v>
       </c>
       <c r="DY15" t="s">
-        <v>3058</v>
+        <v>3062</v>
       </c>
       <c r="DZ15" t="s">
         <v>172</v>
@@ -14381,13 +14393,13 @@
         <v>172</v>
       </c>
       <c r="DA16" t="s">
-        <v>2791</v>
+        <v>2794</v>
       </c>
       <c r="DB16" t="s">
         <v>172</v>
       </c>
       <c r="DC16" t="s">
-        <v>2851</v>
+        <v>2855</v>
       </c>
       <c r="DD16" t="s">
         <v>172</v>
@@ -14399,19 +14411,19 @@
         <v>172</v>
       </c>
       <c r="DK16" t="s">
-        <v>2791</v>
+        <v>2794</v>
       </c>
       <c r="DL16" t="s">
         <v>172</v>
       </c>
       <c r="DW16" t="s">
-        <v>3046</v>
+        <v>3050</v>
       </c>
       <c r="DX16" t="s">
         <v>172</v>
       </c>
       <c r="DY16" t="s">
-        <v>3059</v>
+        <v>3063</v>
       </c>
       <c r="DZ16" t="s">
         <v>172</v>
@@ -14539,13 +14551,13 @@
         <v>172</v>
       </c>
       <c r="DA17" t="s">
-        <v>2792</v>
+        <v>2795</v>
       </c>
       <c r="DB17" t="s">
         <v>172</v>
       </c>
       <c r="DC17" t="s">
-        <v>2852</v>
+        <v>2856</v>
       </c>
       <c r="DD17" t="s">
         <v>172</v>
@@ -14557,7 +14569,7 @@
         <v>172</v>
       </c>
       <c r="DK17" t="s">
-        <v>2792</v>
+        <v>2795</v>
       </c>
       <c r="DL17" t="s">
         <v>172</v>
@@ -14569,7 +14581,7 @@
         <v>172</v>
       </c>
       <c r="DY17" t="s">
-        <v>3060</v>
+        <v>3064</v>
       </c>
       <c r="DZ17" t="s">
         <v>172</v>
@@ -14679,13 +14691,13 @@
         <v>172</v>
       </c>
       <c r="DA18" t="s">
-        <v>2793</v>
+        <v>2796</v>
       </c>
       <c r="DB18" t="s">
         <v>172</v>
       </c>
       <c r="DC18" t="s">
-        <v>2853</v>
+        <v>2857</v>
       </c>
       <c r="DD18" t="s">
         <v>172</v>
@@ -14697,13 +14709,13 @@
         <v>172</v>
       </c>
       <c r="DK18" t="s">
-        <v>2793</v>
+        <v>2796</v>
       </c>
       <c r="DL18" t="s">
         <v>172</v>
       </c>
       <c r="DY18" t="s">
-        <v>3061</v>
+        <v>3065</v>
       </c>
       <c r="DZ18" t="s">
         <v>172</v>
@@ -14807,7 +14819,7 @@
         <v>172</v>
       </c>
       <c r="DA19" t="s">
-        <v>2794</v>
+        <v>2797</v>
       </c>
       <c r="DB19" t="s">
         <v>172</v>
@@ -14825,13 +14837,13 @@
         <v>172</v>
       </c>
       <c r="DK19" t="s">
-        <v>2794</v>
+        <v>2797</v>
       </c>
       <c r="DL19" t="s">
         <v>172</v>
       </c>
       <c r="DY19" t="s">
-        <v>3062</v>
+        <v>3066</v>
       </c>
       <c r="DZ19" t="s">
         <v>172</v>
@@ -14935,13 +14947,13 @@
         <v>172</v>
       </c>
       <c r="DA20" t="s">
-        <v>2795</v>
+        <v>2798</v>
       </c>
       <c r="DB20" t="s">
         <v>172</v>
       </c>
       <c r="DC20" t="s">
-        <v>2854</v>
+        <v>2858</v>
       </c>
       <c r="DD20" t="s">
         <v>172</v>
@@ -14953,13 +14965,13 @@
         <v>172</v>
       </c>
       <c r="DK20" t="s">
-        <v>2795</v>
+        <v>2798</v>
       </c>
       <c r="DL20" t="s">
         <v>172</v>
       </c>
       <c r="DY20" t="s">
-        <v>3063</v>
+        <v>3067</v>
       </c>
       <c r="DZ20" t="s">
         <v>172</v>
@@ -15039,13 +15051,13 @@
         <v>172</v>
       </c>
       <c r="DA21" t="s">
-        <v>2796</v>
+        <v>2799</v>
       </c>
       <c r="DB21" t="s">
         <v>172</v>
       </c>
       <c r="DC21" t="s">
-        <v>2855</v>
+        <v>2859</v>
       </c>
       <c r="DD21" t="s">
         <v>172</v>
@@ -15057,13 +15069,13 @@
         <v>172</v>
       </c>
       <c r="DK21" t="s">
-        <v>2796</v>
+        <v>2799</v>
       </c>
       <c r="DL21" t="s">
         <v>172</v>
       </c>
       <c r="DY21" t="s">
-        <v>3064</v>
+        <v>3068</v>
       </c>
       <c r="DZ21" t="s">
         <v>172</v>
@@ -15143,13 +15155,13 @@
         <v>172</v>
       </c>
       <c r="DA22" t="s">
-        <v>2797</v>
+        <v>2800</v>
       </c>
       <c r="DB22" t="s">
         <v>172</v>
       </c>
       <c r="DC22" t="s">
-        <v>2856</v>
+        <v>2860</v>
       </c>
       <c r="DD22" t="s">
         <v>172</v>
@@ -15161,13 +15173,13 @@
         <v>172</v>
       </c>
       <c r="DK22" t="s">
-        <v>2797</v>
+        <v>2800</v>
       </c>
       <c r="DL22" t="s">
         <v>172</v>
       </c>
       <c r="DY22" t="s">
-        <v>3065</v>
+        <v>3069</v>
       </c>
       <c r="DZ22" t="s">
         <v>172</v>
@@ -15247,13 +15259,13 @@
         <v>172</v>
       </c>
       <c r="DA23" t="s">
-        <v>2258</v>
+        <v>2801</v>
       </c>
       <c r="DB23" t="s">
         <v>172</v>
       </c>
       <c r="DC23" t="s">
-        <v>2857</v>
+        <v>2861</v>
       </c>
       <c r="DD23" t="s">
         <v>172</v>
@@ -15265,7 +15277,7 @@
         <v>172</v>
       </c>
       <c r="DK23" t="s">
-        <v>2258</v>
+        <v>2801</v>
       </c>
       <c r="DL23" t="s">
         <v>172</v>
@@ -15339,13 +15351,13 @@
         <v>172</v>
       </c>
       <c r="DA24" t="s">
-        <v>2798</v>
+        <v>2258</v>
       </c>
       <c r="DB24" t="s">
         <v>172</v>
       </c>
       <c r="DC24" t="s">
-        <v>2858</v>
+        <v>2862</v>
       </c>
       <c r="DD24" t="s">
         <v>172</v>
@@ -15357,13 +15369,13 @@
         <v>172</v>
       </c>
       <c r="DK24" t="s">
-        <v>2798</v>
+        <v>2258</v>
       </c>
       <c r="DL24" t="s">
         <v>172</v>
       </c>
       <c r="DY24" t="s">
-        <v>3066</v>
+        <v>3070</v>
       </c>
       <c r="DZ24" t="s">
         <v>172</v>
@@ -15431,13 +15443,13 @@
         <v>172</v>
       </c>
       <c r="DA25" t="s">
-        <v>2799</v>
+        <v>2802</v>
       </c>
       <c r="DB25" t="s">
         <v>172</v>
       </c>
       <c r="DC25" t="s">
-        <v>2859</v>
+        <v>2863</v>
       </c>
       <c r="DD25" t="s">
         <v>172</v>
@@ -15449,13 +15461,13 @@
         <v>172</v>
       </c>
       <c r="DK25" t="s">
-        <v>2799</v>
+        <v>2802</v>
       </c>
       <c r="DL25" t="s">
         <v>172</v>
       </c>
       <c r="DY25" t="s">
-        <v>3067</v>
+        <v>3071</v>
       </c>
       <c r="DZ25" t="s">
         <v>172</v>
@@ -15517,13 +15529,13 @@
         <v>172</v>
       </c>
       <c r="DA26" t="s">
-        <v>2800</v>
+        <v>2803</v>
       </c>
       <c r="DB26" t="s">
         <v>172</v>
       </c>
       <c r="DC26" t="s">
-        <v>2860</v>
+        <v>2864</v>
       </c>
       <c r="DD26" t="s">
         <v>172</v>
@@ -15535,13 +15547,13 @@
         <v>172</v>
       </c>
       <c r="DK26" t="s">
-        <v>2800</v>
+        <v>2803</v>
       </c>
       <c r="DL26" t="s">
         <v>172</v>
       </c>
       <c r="DY26" t="s">
-        <v>3068</v>
+        <v>3072</v>
       </c>
       <c r="DZ26" t="s">
         <v>172</v>
@@ -15603,13 +15615,13 @@
         <v>172</v>
       </c>
       <c r="DA27" t="s">
-        <v>2801</v>
+        <v>2804</v>
       </c>
       <c r="DB27" t="s">
         <v>172</v>
       </c>
       <c r="DC27" t="s">
-        <v>2861</v>
+        <v>2865</v>
       </c>
       <c r="DD27" t="s">
         <v>172</v>
@@ -15621,13 +15633,13 @@
         <v>172</v>
       </c>
       <c r="DK27" t="s">
-        <v>2801</v>
+        <v>2804</v>
       </c>
       <c r="DL27" t="s">
         <v>172</v>
       </c>
       <c r="DY27" t="s">
-        <v>3069</v>
+        <v>3073</v>
       </c>
       <c r="DZ27" t="s">
         <v>172</v>
@@ -15689,13 +15701,13 @@
         <v>172</v>
       </c>
       <c r="DA28" t="s">
-        <v>2802</v>
+        <v>2805</v>
       </c>
       <c r="DB28" t="s">
         <v>172</v>
       </c>
       <c r="DC28" t="s">
-        <v>2862</v>
+        <v>2866</v>
       </c>
       <c r="DD28" t="s">
         <v>172</v>
@@ -15707,7 +15719,7 @@
         <v>172</v>
       </c>
       <c r="DK28" t="s">
-        <v>2802</v>
+        <v>2805</v>
       </c>
       <c r="DL28" t="s">
         <v>172</v>
@@ -15769,13 +15781,13 @@
         <v>172</v>
       </c>
       <c r="DA29" t="s">
-        <v>2803</v>
+        <v>2806</v>
       </c>
       <c r="DB29" t="s">
         <v>172</v>
       </c>
       <c r="DC29" t="s">
-        <v>2863</v>
+        <v>2867</v>
       </c>
       <c r="DD29" t="s">
         <v>172</v>
@@ -15787,7 +15799,7 @@
         <v>172</v>
       </c>
       <c r="DK29" t="s">
-        <v>2803</v>
+        <v>2806</v>
       </c>
       <c r="DL29" t="s">
         <v>172</v>
@@ -15849,13 +15861,13 @@
         <v>172</v>
       </c>
       <c r="DA30" t="s">
-        <v>2804</v>
+        <v>2807</v>
       </c>
       <c r="DB30" t="s">
         <v>172</v>
       </c>
       <c r="DC30" t="s">
-        <v>2864</v>
+        <v>2868</v>
       </c>
       <c r="DD30" t="s">
         <v>172</v>
@@ -15867,7 +15879,7 @@
         <v>172</v>
       </c>
       <c r="DK30" t="s">
-        <v>2804</v>
+        <v>2807</v>
       </c>
       <c r="DL30" t="s">
         <v>172</v>
@@ -15929,13 +15941,13 @@
         <v>172</v>
       </c>
       <c r="DA31" t="s">
-        <v>2805</v>
+        <v>2808</v>
       </c>
       <c r="DB31" t="s">
         <v>172</v>
       </c>
       <c r="DC31" t="s">
-        <v>2865</v>
+        <v>2869</v>
       </c>
       <c r="DD31" t="s">
         <v>172</v>
@@ -15947,7 +15959,7 @@
         <v>172</v>
       </c>
       <c r="DK31" t="s">
-        <v>2805</v>
+        <v>2808</v>
       </c>
       <c r="DL31" t="s">
         <v>172</v>
@@ -16009,13 +16021,13 @@
         <v>172</v>
       </c>
       <c r="DA32" t="s">
-        <v>2806</v>
+        <v>2809</v>
       </c>
       <c r="DB32" t="s">
         <v>172</v>
       </c>
       <c r="DC32" t="s">
-        <v>2866</v>
+        <v>2870</v>
       </c>
       <c r="DD32" t="s">
         <v>172</v>
@@ -16027,7 +16039,7 @@
         <v>172</v>
       </c>
       <c r="DK32" t="s">
-        <v>2806</v>
+        <v>2809</v>
       </c>
       <c r="DL32" t="s">
         <v>172</v>
@@ -16089,13 +16101,13 @@
         <v>172</v>
       </c>
       <c r="DA33" t="s">
-        <v>2807</v>
+        <v>2810</v>
       </c>
       <c r="DB33" t="s">
         <v>172</v>
       </c>
       <c r="DC33" t="s">
-        <v>2867</v>
+        <v>2871</v>
       </c>
       <c r="DD33" t="s">
         <v>172</v>
@@ -16107,7 +16119,7 @@
         <v>172</v>
       </c>
       <c r="DK33" t="s">
-        <v>2807</v>
+        <v>2810</v>
       </c>
       <c r="DL33" t="s">
         <v>172</v>
@@ -16169,13 +16181,13 @@
         <v>172</v>
       </c>
       <c r="DA34" t="s">
-        <v>2808</v>
+        <v>2811</v>
       </c>
       <c r="DB34" t="s">
         <v>172</v>
       </c>
       <c r="DC34" t="s">
-        <v>2868</v>
+        <v>2872</v>
       </c>
       <c r="DD34" t="s">
         <v>172</v>
@@ -16187,7 +16199,7 @@
         <v>172</v>
       </c>
       <c r="DK34" t="s">
-        <v>2808</v>
+        <v>2811</v>
       </c>
       <c r="DL34" t="s">
         <v>172</v>
@@ -16249,13 +16261,13 @@
         <v>172</v>
       </c>
       <c r="DA35" t="s">
-        <v>2809</v>
+        <v>2812</v>
       </c>
       <c r="DB35" t="s">
         <v>172</v>
       </c>
       <c r="DC35" t="s">
-        <v>2869</v>
+        <v>2873</v>
       </c>
       <c r="DD35" t="s">
         <v>172</v>
@@ -16267,7 +16279,7 @@
         <v>172</v>
       </c>
       <c r="DK35" t="s">
-        <v>2809</v>
+        <v>2812</v>
       </c>
       <c r="DL35" t="s">
         <v>172</v>
@@ -16329,13 +16341,13 @@
         <v>172</v>
       </c>
       <c r="DA36" t="s">
-        <v>2810</v>
+        <v>2813</v>
       </c>
       <c r="DB36" t="s">
         <v>172</v>
       </c>
       <c r="DC36" t="s">
-        <v>2870</v>
+        <v>2874</v>
       </c>
       <c r="DD36" t="s">
         <v>172</v>
@@ -16347,7 +16359,7 @@
         <v>172</v>
       </c>
       <c r="DK36" t="s">
-        <v>2810</v>
+        <v>2813</v>
       </c>
       <c r="DL36" t="s">
         <v>172</v>
@@ -16409,13 +16421,13 @@
         <v>172</v>
       </c>
       <c r="DA37" t="s">
-        <v>2811</v>
+        <v>2814</v>
       </c>
       <c r="DB37" t="s">
         <v>172</v>
       </c>
       <c r="DC37" t="s">
-        <v>2871</v>
+        <v>2875</v>
       </c>
       <c r="DD37" t="s">
         <v>172</v>
@@ -16427,7 +16439,7 @@
         <v>172</v>
       </c>
       <c r="DK37" t="s">
-        <v>2811</v>
+        <v>2814</v>
       </c>
       <c r="DL37" t="s">
         <v>172</v>
@@ -16489,13 +16501,13 @@
         <v>172</v>
       </c>
       <c r="DA38" t="s">
-        <v>2812</v>
+        <v>2815</v>
       </c>
       <c r="DB38" t="s">
         <v>172</v>
       </c>
       <c r="DC38" t="s">
-        <v>2872</v>
+        <v>2876</v>
       </c>
       <c r="DD38" t="s">
         <v>172</v>
@@ -16507,7 +16519,7 @@
         <v>172</v>
       </c>
       <c r="DK38" t="s">
-        <v>2812</v>
+        <v>2815</v>
       </c>
       <c r="DL38" t="s">
         <v>172</v>
@@ -16569,13 +16581,13 @@
         <v>172</v>
       </c>
       <c r="DA39" t="s">
-        <v>2813</v>
+        <v>2816</v>
       </c>
       <c r="DB39" t="s">
         <v>172</v>
       </c>
       <c r="DC39" t="s">
-        <v>2873</v>
+        <v>2877</v>
       </c>
       <c r="DD39" t="s">
         <v>172</v>
@@ -16587,7 +16599,7 @@
         <v>172</v>
       </c>
       <c r="DK39" t="s">
-        <v>2813</v>
+        <v>2816</v>
       </c>
       <c r="DL39" t="s">
         <v>172</v>
@@ -16649,13 +16661,13 @@
         <v>172</v>
       </c>
       <c r="DA40" t="s">
-        <v>2814</v>
+        <v>2817</v>
       </c>
       <c r="DB40" t="s">
         <v>172</v>
       </c>
       <c r="DC40" t="s">
-        <v>2874</v>
+        <v>2878</v>
       </c>
       <c r="DD40" t="s">
         <v>172</v>
@@ -16667,7 +16679,7 @@
         <v>172</v>
       </c>
       <c r="DK40" t="s">
-        <v>2814</v>
+        <v>2817</v>
       </c>
       <c r="DL40" t="s">
         <v>172</v>
@@ -16729,13 +16741,13 @@
         <v>172</v>
       </c>
       <c r="DA41" t="s">
-        <v>2815</v>
+        <v>2818</v>
       </c>
       <c r="DB41" t="s">
         <v>172</v>
       </c>
       <c r="DC41" t="s">
-        <v>2875</v>
+        <v>2879</v>
       </c>
       <c r="DD41" t="s">
         <v>172</v>
@@ -16747,7 +16759,7 @@
         <v>172</v>
       </c>
       <c r="DK41" t="s">
-        <v>2815</v>
+        <v>2818</v>
       </c>
       <c r="DL41" t="s">
         <v>172</v>
@@ -16809,13 +16821,13 @@
         <v>172</v>
       </c>
       <c r="DA42" t="s">
-        <v>2816</v>
+        <v>2819</v>
       </c>
       <c r="DB42" t="s">
         <v>172</v>
       </c>
       <c r="DC42" t="s">
-        <v>2876</v>
+        <v>2880</v>
       </c>
       <c r="DD42" t="s">
         <v>172</v>
@@ -16827,7 +16839,7 @@
         <v>172</v>
       </c>
       <c r="DK42" t="s">
-        <v>2816</v>
+        <v>2819</v>
       </c>
       <c r="DL42" t="s">
         <v>172</v>
@@ -16889,13 +16901,13 @@
         <v>172</v>
       </c>
       <c r="DA43" t="s">
-        <v>2817</v>
+        <v>2820</v>
       </c>
       <c r="DB43" t="s">
         <v>172</v>
       </c>
       <c r="DC43" t="s">
-        <v>2877</v>
+        <v>2881</v>
       </c>
       <c r="DD43" t="s">
         <v>172</v>
@@ -16907,7 +16919,7 @@
         <v>172</v>
       </c>
       <c r="DK43" t="s">
-        <v>2817</v>
+        <v>2820</v>
       </c>
       <c r="DL43" t="s">
         <v>172</v>
@@ -16969,13 +16981,13 @@
         <v>172</v>
       </c>
       <c r="DA44" t="s">
-        <v>2818</v>
+        <v>2821</v>
       </c>
       <c r="DB44" t="s">
         <v>172</v>
       </c>
       <c r="DC44" t="s">
-        <v>2878</v>
+        <v>2882</v>
       </c>
       <c r="DD44" t="s">
         <v>172</v>
@@ -16987,7 +16999,7 @@
         <v>172</v>
       </c>
       <c r="DK44" t="s">
-        <v>2818</v>
+        <v>2821</v>
       </c>
       <c r="DL44" t="s">
         <v>172</v>
@@ -17049,13 +17061,13 @@
         <v>172</v>
       </c>
       <c r="DA45" t="s">
-        <v>2819</v>
+        <v>2822</v>
       </c>
       <c r="DB45" t="s">
         <v>172</v>
       </c>
       <c r="DC45" t="s">
-        <v>2879</v>
+        <v>2883</v>
       </c>
       <c r="DD45" t="s">
         <v>172</v>
@@ -17067,7 +17079,7 @@
         <v>172</v>
       </c>
       <c r="DK45" t="s">
-        <v>2819</v>
+        <v>2822</v>
       </c>
       <c r="DL45" t="s">
         <v>172</v>
@@ -17129,13 +17141,13 @@
         <v>172</v>
       </c>
       <c r="DA46" t="s">
-        <v>2820</v>
+        <v>2823</v>
       </c>
       <c r="DB46" t="s">
         <v>172</v>
       </c>
       <c r="DC46" t="s">
-        <v>2880</v>
+        <v>2884</v>
       </c>
       <c r="DD46" t="s">
         <v>172</v>
@@ -17147,7 +17159,7 @@
         <v>172</v>
       </c>
       <c r="DK46" t="s">
-        <v>2820</v>
+        <v>2823</v>
       </c>
       <c r="DL46" t="s">
         <v>172</v>
@@ -17209,13 +17221,13 @@
         <v>172</v>
       </c>
       <c r="DA47" t="s">
-        <v>2821</v>
+        <v>2824</v>
       </c>
       <c r="DB47" t="s">
         <v>172</v>
       </c>
       <c r="DC47" t="s">
-        <v>2881</v>
+        <v>2885</v>
       </c>
       <c r="DD47" t="s">
         <v>172</v>
@@ -17227,7 +17239,7 @@
         <v>172</v>
       </c>
       <c r="DK47" t="s">
-        <v>2821</v>
+        <v>2824</v>
       </c>
       <c r="DL47" t="s">
         <v>172</v>
@@ -17289,13 +17301,13 @@
         <v>172</v>
       </c>
       <c r="DA48" t="s">
-        <v>2822</v>
+        <v>2825</v>
       </c>
       <c r="DB48" t="s">
         <v>172</v>
       </c>
       <c r="DC48" t="s">
-        <v>2882</v>
+        <v>2886</v>
       </c>
       <c r="DD48" t="s">
         <v>172</v>
@@ -17307,7 +17319,7 @@
         <v>172</v>
       </c>
       <c r="DK48" t="s">
-        <v>2822</v>
+        <v>2825</v>
       </c>
       <c r="DL48" t="s">
         <v>172</v>
@@ -17369,13 +17381,13 @@
         <v>172</v>
       </c>
       <c r="DA49" t="s">
-        <v>2823</v>
+        <v>2826</v>
       </c>
       <c r="DB49" t="s">
         <v>172</v>
       </c>
       <c r="DC49" t="s">
-        <v>2883</v>
+        <v>2887</v>
       </c>
       <c r="DD49" t="s">
         <v>172</v>
@@ -17387,7 +17399,7 @@
         <v>172</v>
       </c>
       <c r="DK49" t="s">
-        <v>2823</v>
+        <v>2826</v>
       </c>
       <c r="DL49" t="s">
         <v>172</v>
@@ -17449,13 +17461,13 @@
         <v>172</v>
       </c>
       <c r="DA50" t="s">
-        <v>2824</v>
+        <v>2827</v>
       </c>
       <c r="DB50" t="s">
         <v>172</v>
       </c>
       <c r="DC50" t="s">
-        <v>2884</v>
+        <v>2888</v>
       </c>
       <c r="DD50" t="s">
         <v>172</v>
@@ -17467,7 +17479,7 @@
         <v>172</v>
       </c>
       <c r="DK50" t="s">
-        <v>2824</v>
+        <v>2827</v>
       </c>
       <c r="DL50" t="s">
         <v>172</v>
@@ -17529,13 +17541,13 @@
         <v>172</v>
       </c>
       <c r="DA51" t="s">
-        <v>2825</v>
+        <v>2828</v>
       </c>
       <c r="DB51" t="s">
         <v>172</v>
       </c>
       <c r="DC51" t="s">
-        <v>2885</v>
+        <v>2889</v>
       </c>
       <c r="DD51" t="s">
         <v>172</v>
@@ -17547,7 +17559,7 @@
         <v>172</v>
       </c>
       <c r="DK51" t="s">
-        <v>2825</v>
+        <v>2828</v>
       </c>
       <c r="DL51" t="s">
         <v>172</v>
@@ -17603,13 +17615,13 @@
         <v>172</v>
       </c>
       <c r="DA52" t="s">
-        <v>211</v>
+        <v>2829</v>
       </c>
       <c r="DB52" t="s">
         <v>172</v>
       </c>
       <c r="DC52" t="s">
-        <v>2886</v>
+        <v>2890</v>
       </c>
       <c r="DD52" t="s">
         <v>172</v>
@@ -17621,7 +17633,7 @@
         <v>172</v>
       </c>
       <c r="DK52" t="s">
-        <v>211</v>
+        <v>2829</v>
       </c>
       <c r="DL52" t="s">
         <v>172</v>
@@ -17677,13 +17689,13 @@
         <v>172</v>
       </c>
       <c r="DA53" t="s">
-        <v>2826</v>
+        <v>211</v>
       </c>
       <c r="DB53" t="s">
         <v>172</v>
       </c>
       <c r="DC53" t="s">
-        <v>2887</v>
+        <v>2891</v>
       </c>
       <c r="DD53" t="s">
         <v>172</v>
@@ -17695,7 +17707,7 @@
         <v>172</v>
       </c>
       <c r="DK53" t="s">
-        <v>2826</v>
+        <v>211</v>
       </c>
       <c r="DL53" t="s">
         <v>172</v>
@@ -17751,13 +17763,13 @@
         <v>172</v>
       </c>
       <c r="DA54" t="s">
-        <v>2827</v>
+        <v>2830</v>
       </c>
       <c r="DB54" t="s">
         <v>172</v>
       </c>
       <c r="DC54" t="s">
-        <v>2888</v>
+        <v>2892</v>
       </c>
       <c r="DD54" t="s">
         <v>172</v>
@@ -17769,7 +17781,7 @@
         <v>172</v>
       </c>
       <c r="DK54" t="s">
-        <v>2827</v>
+        <v>2830</v>
       </c>
       <c r="DL54" t="s">
         <v>172</v>
@@ -17825,13 +17837,13 @@
         <v>172</v>
       </c>
       <c r="DA55" t="s">
-        <v>2828</v>
+        <v>2831</v>
       </c>
       <c r="DB55" t="s">
         <v>172</v>
       </c>
       <c r="DC55" t="s">
-        <v>2889</v>
+        <v>2893</v>
       </c>
       <c r="DD55" t="s">
         <v>172</v>
@@ -17843,7 +17855,7 @@
         <v>172</v>
       </c>
       <c r="DK55" t="s">
-        <v>2828</v>
+        <v>2831</v>
       </c>
       <c r="DL55" t="s">
         <v>172</v>
@@ -17899,13 +17911,13 @@
         <v>172</v>
       </c>
       <c r="DA56" t="s">
-        <v>2829</v>
+        <v>2832</v>
       </c>
       <c r="DB56" t="s">
         <v>172</v>
       </c>
       <c r="DC56" t="s">
-        <v>2890</v>
+        <v>2894</v>
       </c>
       <c r="DD56" t="s">
         <v>172</v>
@@ -17917,7 +17929,7 @@
         <v>172</v>
       </c>
       <c r="DK56" t="s">
-        <v>2829</v>
+        <v>2832</v>
       </c>
       <c r="DL56" t="s">
         <v>172</v>
@@ -17973,13 +17985,13 @@
         <v>172</v>
       </c>
       <c r="DA57" t="s">
-        <v>2830</v>
+        <v>2833</v>
       </c>
       <c r="DB57" t="s">
         <v>172</v>
       </c>
       <c r="DC57" t="s">
-        <v>2891</v>
+        <v>2895</v>
       </c>
       <c r="DD57" t="s">
         <v>172</v>
@@ -17991,7 +18003,7 @@
         <v>172</v>
       </c>
       <c r="DK57" t="s">
-        <v>2830</v>
+        <v>2833</v>
       </c>
       <c r="DL57" t="s">
         <v>172</v>
@@ -18047,13 +18059,13 @@
         <v>172</v>
       </c>
       <c r="DA58" t="s">
-        <v>2831</v>
+        <v>2834</v>
       </c>
       <c r="DB58" t="s">
         <v>172</v>
       </c>
       <c r="DC58" t="s">
-        <v>2892</v>
+        <v>2896</v>
       </c>
       <c r="DD58" t="s">
         <v>172</v>
@@ -18065,7 +18077,7 @@
         <v>172</v>
       </c>
       <c r="DK58" t="s">
-        <v>2831</v>
+        <v>2834</v>
       </c>
       <c r="DL58" t="s">
         <v>172</v>
@@ -18121,13 +18133,13 @@
         <v>172</v>
       </c>
       <c r="DA59" t="s">
-        <v>2832</v>
+        <v>2835</v>
       </c>
       <c r="DB59" t="s">
         <v>172</v>
       </c>
       <c r="DC59" t="s">
-        <v>2893</v>
+        <v>2897</v>
       </c>
       <c r="DD59" t="s">
         <v>172</v>
@@ -18139,7 +18151,7 @@
         <v>172</v>
       </c>
       <c r="DK59" t="s">
-        <v>2832</v>
+        <v>2835</v>
       </c>
       <c r="DL59" t="s">
         <v>172</v>
@@ -18195,7 +18207,7 @@
         <v>172</v>
       </c>
       <c r="DA60" t="s">
-        <v>2833</v>
+        <v>2836</v>
       </c>
       <c r="DB60" t="s">
         <v>172</v>
@@ -18213,7 +18225,7 @@
         <v>172</v>
       </c>
       <c r="DK60" t="s">
-        <v>2833</v>
+        <v>2836</v>
       </c>
       <c r="DL60" t="s">
         <v>172</v>
@@ -18251,13 +18263,13 @@
         <v>172</v>
       </c>
       <c r="DA61" t="s">
-        <v>2834</v>
+        <v>2837</v>
       </c>
       <c r="DB61" t="s">
         <v>172</v>
       </c>
       <c r="DC61" t="s">
-        <v>2894</v>
+        <v>2898</v>
       </c>
       <c r="DD61" t="s">
         <v>172</v>
@@ -18269,7 +18281,7 @@
         <v>172</v>
       </c>
       <c r="DK61" t="s">
-        <v>2834</v>
+        <v>2837</v>
       </c>
       <c r="DL61" t="s">
         <v>172</v>
@@ -18301,13 +18313,13 @@
         <v>172</v>
       </c>
       <c r="DA62" t="s">
-        <v>2835</v>
+        <v>2838</v>
       </c>
       <c r="DB62" t="s">
         <v>172</v>
       </c>
       <c r="DC62" t="s">
-        <v>2895</v>
+        <v>2899</v>
       </c>
       <c r="DD62" t="s">
         <v>172</v>
@@ -18319,7 +18331,7 @@
         <v>172</v>
       </c>
       <c r="DK62" t="s">
-        <v>2835</v>
+        <v>2838</v>
       </c>
       <c r="DL62" t="s">
         <v>172</v>
@@ -18351,13 +18363,13 @@
         <v>172</v>
       </c>
       <c r="DA63" t="s">
-        <v>2553</v>
+        <v>2839</v>
       </c>
       <c r="DB63" t="s">
         <v>172</v>
       </c>
       <c r="DC63" t="s">
-        <v>2896</v>
+        <v>2900</v>
       </c>
       <c r="DD63" t="s">
         <v>172</v>
@@ -18369,7 +18381,7 @@
         <v>172</v>
       </c>
       <c r="DK63" t="s">
-        <v>2553</v>
+        <v>2839</v>
       </c>
       <c r="DL63" t="s">
         <v>172</v>
@@ -18401,13 +18413,13 @@
         <v>172</v>
       </c>
       <c r="DA64" t="s">
-        <v>2836</v>
+        <v>2553</v>
       </c>
       <c r="DB64" t="s">
         <v>172</v>
       </c>
       <c r="DC64" t="s">
-        <v>2897</v>
+        <v>2901</v>
       </c>
       <c r="DD64" t="s">
         <v>172</v>
@@ -18419,7 +18431,7 @@
         <v>172</v>
       </c>
       <c r="DK64" t="s">
-        <v>2836</v>
+        <v>2553</v>
       </c>
       <c r="DL64" t="s">
         <v>172</v>
@@ -18451,13 +18463,13 @@
         <v>172</v>
       </c>
       <c r="DA65" t="s">
-        <v>2837</v>
+        <v>2840</v>
       </c>
       <c r="DB65" t="s">
         <v>172</v>
       </c>
       <c r="DC65" t="s">
-        <v>2898</v>
+        <v>2902</v>
       </c>
       <c r="DD65" t="s">
         <v>172</v>
@@ -18469,7 +18481,7 @@
         <v>172</v>
       </c>
       <c r="DK65" t="s">
-        <v>2837</v>
+        <v>2840</v>
       </c>
       <c r="DL65" t="s">
         <v>172</v>
@@ -18501,13 +18513,13 @@
         <v>172</v>
       </c>
       <c r="DA66" t="s">
-        <v>2838</v>
+        <v>2841</v>
       </c>
       <c r="DB66" t="s">
         <v>172</v>
       </c>
       <c r="DC66" t="s">
-        <v>2899</v>
+        <v>2903</v>
       </c>
       <c r="DD66" t="s">
         <v>172</v>
@@ -18519,7 +18531,7 @@
         <v>172</v>
       </c>
       <c r="DK66" t="s">
-        <v>2838</v>
+        <v>2841</v>
       </c>
       <c r="DL66" t="s">
         <v>172</v>
@@ -18550,8 +18562,14 @@
       <c r="CZ67" t="s">
         <v>172</v>
       </c>
+      <c r="DA67" t="s">
+        <v>2842</v>
+      </c>
+      <c r="DB67" t="s">
+        <v>172</v>
+      </c>
       <c r="DC67" t="s">
-        <v>2900</v>
+        <v>2904</v>
       </c>
       <c r="DD67" t="s">
         <v>172</v>
@@ -18560,6 +18578,12 @@
         <v>1940</v>
       </c>
       <c r="DJ67" t="s">
+        <v>172</v>
+      </c>
+      <c r="DK67" t="s">
+        <v>2842</v>
+      </c>
+      <c r="DL67" t="s">
         <v>172</v>
       </c>
     </row>
@@ -18589,7 +18613,7 @@
         <v>172</v>
       </c>
       <c r="DC68" t="s">
-        <v>2901</v>
+        <v>2905</v>
       </c>
       <c r="DD68" t="s">
         <v>172</v>
@@ -18627,7 +18651,7 @@
         <v>172</v>
       </c>
       <c r="DC69" t="s">
-        <v>2902</v>
+        <v>2906</v>
       </c>
       <c r="DD69" t="s">
         <v>172</v>
@@ -18665,7 +18689,7 @@
         <v>172</v>
       </c>
       <c r="DC70" t="s">
-        <v>2903</v>
+        <v>2907</v>
       </c>
       <c r="DD70" t="s">
         <v>172</v>
@@ -18703,7 +18727,7 @@
         <v>172</v>
       </c>
       <c r="DC71" t="s">
-        <v>2904</v>
+        <v>2908</v>
       </c>
       <c r="DD71" t="s">
         <v>172</v>
@@ -18741,7 +18765,7 @@
         <v>172</v>
       </c>
       <c r="DC72" t="s">
-        <v>2905</v>
+        <v>2909</v>
       </c>
       <c r="DD72" t="s">
         <v>172</v>
@@ -18779,7 +18803,7 @@
         <v>172</v>
       </c>
       <c r="DC73" t="s">
-        <v>2906</v>
+        <v>2910</v>
       </c>
       <c r="DD73" t="s">
         <v>172</v>
@@ -18817,7 +18841,7 @@
         <v>172</v>
       </c>
       <c r="DC74" t="s">
-        <v>2907</v>
+        <v>2911</v>
       </c>
       <c r="DD74" t="s">
         <v>172</v>
@@ -18855,7 +18879,7 @@
         <v>172</v>
       </c>
       <c r="DC75" t="s">
-        <v>2908</v>
+        <v>2912</v>
       </c>
       <c r="DD75" t="s">
         <v>172</v>
@@ -18893,7 +18917,7 @@
         <v>172</v>
       </c>
       <c r="DC76" t="s">
-        <v>2909</v>
+        <v>2913</v>
       </c>
       <c r="DD76" t="s">
         <v>172</v>
@@ -18931,7 +18955,7 @@
         <v>172</v>
       </c>
       <c r="DC77" t="s">
-        <v>2910</v>
+        <v>2914</v>
       </c>
       <c r="DD77" t="s">
         <v>172</v>
@@ -18969,7 +18993,7 @@
         <v>172</v>
       </c>
       <c r="DC78" t="s">
-        <v>2911</v>
+        <v>2915</v>
       </c>
       <c r="DD78" t="s">
         <v>172</v>
@@ -19007,7 +19031,7 @@
         <v>172</v>
       </c>
       <c r="DC79" t="s">
-        <v>2912</v>
+        <v>2916</v>
       </c>
       <c r="DD79" t="s">
         <v>172</v>
@@ -19045,7 +19069,7 @@
         <v>172</v>
       </c>
       <c r="DC80" t="s">
-        <v>2913</v>
+        <v>2917</v>
       </c>
       <c r="DD80" t="s">
         <v>172</v>
@@ -19083,7 +19107,7 @@
         <v>172</v>
       </c>
       <c r="DC81" t="s">
-        <v>2914</v>
+        <v>2918</v>
       </c>
       <c r="DD81" t="s">
         <v>172</v>
@@ -19121,7 +19145,7 @@
         <v>172</v>
       </c>
       <c r="DC82" t="s">
-        <v>2915</v>
+        <v>2919</v>
       </c>
       <c r="DD82" t="s">
         <v>172</v>
@@ -19159,7 +19183,7 @@
         <v>172</v>
       </c>
       <c r="DC83" t="s">
-        <v>2916</v>
+        <v>2920</v>
       </c>
       <c r="DD83" t="s">
         <v>172</v>
@@ -19197,7 +19221,7 @@
         <v>172</v>
       </c>
       <c r="DC84" t="s">
-        <v>2917</v>
+        <v>2921</v>
       </c>
       <c r="DD84" t="s">
         <v>172</v>
@@ -19235,7 +19259,7 @@
         <v>172</v>
       </c>
       <c r="DC85" t="s">
-        <v>2918</v>
+        <v>2922</v>
       </c>
       <c r="DD85" t="s">
         <v>172</v>
@@ -19273,7 +19297,7 @@
         <v>172</v>
       </c>
       <c r="DC86" t="s">
-        <v>2919</v>
+        <v>2923</v>
       </c>
       <c r="DD86" t="s">
         <v>172</v>
@@ -19311,7 +19335,7 @@
         <v>172</v>
       </c>
       <c r="DC87" t="s">
-        <v>2920</v>
+        <v>2924</v>
       </c>
       <c r="DD87" t="s">
         <v>172</v>
@@ -19349,7 +19373,7 @@
         <v>172</v>
       </c>
       <c r="DC88" t="s">
-        <v>2921</v>
+        <v>2925</v>
       </c>
       <c r="DD88" t="s">
         <v>172</v>
@@ -19387,7 +19411,7 @@
         <v>172</v>
       </c>
       <c r="DC89" t="s">
-        <v>2922</v>
+        <v>2926</v>
       </c>
       <c r="DD89" t="s">
         <v>172</v>
@@ -19425,7 +19449,7 @@
         <v>172</v>
       </c>
       <c r="DC90" t="s">
-        <v>2923</v>
+        <v>2927</v>
       </c>
       <c r="DD90" t="s">
         <v>172</v>
@@ -19463,7 +19487,7 @@
         <v>172</v>
       </c>
       <c r="DC91" t="s">
-        <v>2924</v>
+        <v>2928</v>
       </c>
       <c r="DD91" t="s">
         <v>172</v>
@@ -19539,7 +19563,7 @@
         <v>172</v>
       </c>
       <c r="DC93" t="s">
-        <v>2925</v>
+        <v>2929</v>
       </c>
       <c r="DD93" t="s">
         <v>172</v>
@@ -19577,7 +19601,7 @@
         <v>172</v>
       </c>
       <c r="DC94" t="s">
-        <v>2926</v>
+        <v>2930</v>
       </c>
       <c r="DD94" t="s">
         <v>172</v>
@@ -19615,7 +19639,7 @@
         <v>172</v>
       </c>
       <c r="DC95" t="s">
-        <v>2927</v>
+        <v>2931</v>
       </c>
       <c r="DD95" t="s">
         <v>172</v>
@@ -19653,7 +19677,7 @@
         <v>172</v>
       </c>
       <c r="DC96" t="s">
-        <v>2928</v>
+        <v>2932</v>
       </c>
       <c r="DD96" t="s">
         <v>172</v>
@@ -19691,7 +19715,7 @@
         <v>172</v>
       </c>
       <c r="DC97" t="s">
-        <v>2929</v>
+        <v>2933</v>
       </c>
       <c r="DD97" t="s">
         <v>172</v>
@@ -19729,7 +19753,7 @@
         <v>172</v>
       </c>
       <c r="DC98" t="s">
-        <v>2930</v>
+        <v>2934</v>
       </c>
       <c r="DD98" t="s">
         <v>172</v>
@@ -19767,7 +19791,7 @@
         <v>172</v>
       </c>
       <c r="DC99" t="s">
-        <v>2931</v>
+        <v>2935</v>
       </c>
       <c r="DD99" t="s">
         <v>172</v>
@@ -19805,7 +19829,7 @@
         <v>172</v>
       </c>
       <c r="DC100" t="s">
-        <v>2932</v>
+        <v>2936</v>
       </c>
       <c r="DD100" t="s">
         <v>172</v>
@@ -19843,7 +19867,7 @@
         <v>172</v>
       </c>
       <c r="DC101" t="s">
-        <v>2933</v>
+        <v>2937</v>
       </c>
       <c r="DD101" t="s">
         <v>172</v>
@@ -19881,7 +19905,7 @@
         <v>172</v>
       </c>
       <c r="DC102" t="s">
-        <v>2934</v>
+        <v>2938</v>
       </c>
       <c r="DD102" t="s">
         <v>172</v>
@@ -19919,7 +19943,7 @@
         <v>172</v>
       </c>
       <c r="DC103" t="s">
-        <v>2935</v>
+        <v>2939</v>
       </c>
       <c r="DD103" t="s">
         <v>172</v>
@@ -19957,7 +19981,7 @@
         <v>172</v>
       </c>
       <c r="DC104" t="s">
-        <v>2936</v>
+        <v>2940</v>
       </c>
       <c r="DD104" t="s">
         <v>172</v>
@@ -19995,7 +20019,7 @@
         <v>172</v>
       </c>
       <c r="DC105" t="s">
-        <v>2937</v>
+        <v>2941</v>
       </c>
       <c r="DD105" t="s">
         <v>172</v>
@@ -20033,7 +20057,7 @@
         <v>172</v>
       </c>
       <c r="DC106" t="s">
-        <v>2938</v>
+        <v>2942</v>
       </c>
       <c r="DD106" t="s">
         <v>172</v>
@@ -20071,7 +20095,7 @@
         <v>172</v>
       </c>
       <c r="DC107" t="s">
-        <v>2939</v>
+        <v>2943</v>
       </c>
       <c r="DD107" t="s">
         <v>172</v>
@@ -20109,7 +20133,7 @@
         <v>172</v>
       </c>
       <c r="DC108" t="s">
-        <v>2940</v>
+        <v>2944</v>
       </c>
       <c r="DD108" t="s">
         <v>172</v>
@@ -20147,7 +20171,7 @@
         <v>172</v>
       </c>
       <c r="DC109" t="s">
-        <v>2941</v>
+        <v>2945</v>
       </c>
       <c r="DD109" t="s">
         <v>172</v>
@@ -20185,7 +20209,7 @@
         <v>172</v>
       </c>
       <c r="DC110" t="s">
-        <v>2942</v>
+        <v>2946</v>
       </c>
       <c r="DD110" t="s">
         <v>172</v>
@@ -20223,7 +20247,7 @@
         <v>172</v>
       </c>
       <c r="DC111" t="s">
-        <v>2943</v>
+        <v>2947</v>
       </c>
       <c r="DD111" t="s">
         <v>172</v>
@@ -20261,7 +20285,7 @@
         <v>172</v>
       </c>
       <c r="DC112" t="s">
-        <v>2944</v>
+        <v>2948</v>
       </c>
       <c r="DD112" t="s">
         <v>172</v>
@@ -20299,7 +20323,7 @@
         <v>172</v>
       </c>
       <c r="DC113" t="s">
-        <v>2945</v>
+        <v>2949</v>
       </c>
       <c r="DD113" t="s">
         <v>172</v>
@@ -20337,7 +20361,7 @@
         <v>172</v>
       </c>
       <c r="DC114" t="s">
-        <v>2946</v>
+        <v>2950</v>
       </c>
       <c r="DD114" t="s">
         <v>172</v>
@@ -20375,7 +20399,7 @@
         <v>172</v>
       </c>
       <c r="DC115" t="s">
-        <v>2947</v>
+        <v>2951</v>
       </c>
       <c r="DD115" t="s">
         <v>172</v>
@@ -20413,7 +20437,7 @@
         <v>172</v>
       </c>
       <c r="DC116" t="s">
-        <v>2948</v>
+        <v>2952</v>
       </c>
       <c r="DD116" t="s">
         <v>172</v>
@@ -20451,7 +20475,7 @@
         <v>172</v>
       </c>
       <c r="DC117" t="s">
-        <v>2949</v>
+        <v>2953</v>
       </c>
       <c r="DD117" t="s">
         <v>172</v>
@@ -20489,7 +20513,7 @@
         <v>172</v>
       </c>
       <c r="DC118" t="s">
-        <v>2950</v>
+        <v>2954</v>
       </c>
       <c r="DD118" t="s">
         <v>172</v>
@@ -20527,7 +20551,7 @@
         <v>172</v>
       </c>
       <c r="DC119" t="s">
-        <v>2951</v>
+        <v>2955</v>
       </c>
       <c r="DD119" t="s">
         <v>172</v>
@@ -20565,7 +20589,7 @@
         <v>172</v>
       </c>
       <c r="DC120" t="s">
-        <v>2952</v>
+        <v>2956</v>
       </c>
       <c r="DD120" t="s">
         <v>172</v>
@@ -20603,7 +20627,7 @@
         <v>172</v>
       </c>
       <c r="DC121" t="s">
-        <v>2953</v>
+        <v>2957</v>
       </c>
       <c r="DD121" t="s">
         <v>172</v>
@@ -20641,7 +20665,7 @@
         <v>172</v>
       </c>
       <c r="DC122" t="s">
-        <v>2954</v>
+        <v>2958</v>
       </c>
       <c r="DD122" t="s">
         <v>172</v>
@@ -20679,7 +20703,7 @@
         <v>172</v>
       </c>
       <c r="DC123" t="s">
-        <v>2955</v>
+        <v>2959</v>
       </c>
       <c r="DD123" t="s">
         <v>172</v>
@@ -20717,7 +20741,7 @@
         <v>172</v>
       </c>
       <c r="DC124" t="s">
-        <v>2956</v>
+        <v>2960</v>
       </c>
       <c r="DD124" t="s">
         <v>172</v>
@@ -20755,7 +20779,7 @@
         <v>172</v>
       </c>
       <c r="DC125" t="s">
-        <v>2957</v>
+        <v>2961</v>
       </c>
       <c r="DD125" t="s">
         <v>172</v>
@@ -20793,7 +20817,7 @@
         <v>172</v>
       </c>
       <c r="DC126" t="s">
-        <v>2958</v>
+        <v>2962</v>
       </c>
       <c r="DD126" t="s">
         <v>172</v>
@@ -20831,7 +20855,7 @@
         <v>172</v>
       </c>
       <c r="DC127" t="s">
-        <v>2959</v>
+        <v>2963</v>
       </c>
       <c r="DD127" t="s">
         <v>172</v>
@@ -20869,7 +20893,7 @@
         <v>172</v>
       </c>
       <c r="DC128" t="s">
-        <v>2960</v>
+        <v>2964</v>
       </c>
       <c r="DD128" t="s">
         <v>172</v>
@@ -20907,7 +20931,7 @@
         <v>172</v>
       </c>
       <c r="DC129" t="s">
-        <v>2961</v>
+        <v>2965</v>
       </c>
       <c r="DD129" t="s">
         <v>172</v>
@@ -20945,7 +20969,7 @@
         <v>172</v>
       </c>
       <c r="DC130" t="s">
-        <v>2962</v>
+        <v>2966</v>
       </c>
       <c r="DD130" t="s">
         <v>172</v>
@@ -20983,7 +21007,7 @@
         <v>172</v>
       </c>
       <c r="DC131" t="s">
-        <v>2963</v>
+        <v>2967</v>
       </c>
       <c r="DD131" t="s">
         <v>172</v>
@@ -21021,7 +21045,7 @@
         <v>172</v>
       </c>
       <c r="DC132" t="s">
-        <v>2964</v>
+        <v>2968</v>
       </c>
       <c r="DD132" t="s">
         <v>172</v>
@@ -21059,7 +21083,7 @@
         <v>172</v>
       </c>
       <c r="DC133" t="s">
-        <v>2965</v>
+        <v>2969</v>
       </c>
       <c r="DD133" t="s">
         <v>172</v>
@@ -21097,7 +21121,7 @@
         <v>172</v>
       </c>
       <c r="DC134" t="s">
-        <v>2966</v>
+        <v>2970</v>
       </c>
       <c r="DD134" t="s">
         <v>172</v>
@@ -21135,7 +21159,7 @@
         <v>172</v>
       </c>
       <c r="DC135" t="s">
-        <v>2967</v>
+        <v>2971</v>
       </c>
       <c r="DD135" t="s">
         <v>172</v>
@@ -21173,7 +21197,7 @@
         <v>172</v>
       </c>
       <c r="DC136" t="s">
-        <v>2968</v>
+        <v>2972</v>
       </c>
       <c r="DD136" t="s">
         <v>172</v>
@@ -21211,7 +21235,7 @@
         <v>172</v>
       </c>
       <c r="DC137" t="s">
-        <v>2969</v>
+        <v>2973</v>
       </c>
       <c r="DD137" t="s">
         <v>172</v>
@@ -21237,7 +21261,7 @@
         <v>172</v>
       </c>
       <c r="DC138" t="s">
-        <v>2970</v>
+        <v>2974</v>
       </c>
       <c r="DD138" t="s">
         <v>172</v>
@@ -21263,7 +21287,7 @@
         <v>172</v>
       </c>
       <c r="DC139" t="s">
-        <v>2971</v>
+        <v>2975</v>
       </c>
       <c r="DD139" t="s">
         <v>172</v>
@@ -21289,7 +21313,7 @@
         <v>172</v>
       </c>
       <c r="DC140" t="s">
-        <v>2972</v>
+        <v>2976</v>
       </c>
       <c r="DD140" t="s">
         <v>172</v>
@@ -21315,7 +21339,7 @@
         <v>172</v>
       </c>
       <c r="DC141" t="s">
-        <v>2973</v>
+        <v>2977</v>
       </c>
       <c r="DD141" t="s">
         <v>172</v>
@@ -21367,7 +21391,7 @@
         <v>172</v>
       </c>
       <c r="DC143" t="s">
-        <v>2974</v>
+        <v>2978</v>
       </c>
       <c r="DD143" t="s">
         <v>172</v>
@@ -21393,7 +21417,7 @@
         <v>172</v>
       </c>
       <c r="DC144" t="s">
-        <v>2975</v>
+        <v>2979</v>
       </c>
       <c r="DD144" t="s">
         <v>172</v>
@@ -21419,7 +21443,7 @@
         <v>172</v>
       </c>
       <c r="DC145" t="s">
-        <v>2976</v>
+        <v>2980</v>
       </c>
       <c r="DD145" t="s">
         <v>172</v>
@@ -21445,7 +21469,7 @@
         <v>172</v>
       </c>
       <c r="DC146" t="s">
-        <v>2977</v>
+        <v>2981</v>
       </c>
       <c r="DD146" t="s">
         <v>172</v>
@@ -21471,7 +21495,7 @@
         <v>172</v>
       </c>
       <c r="DC147" t="s">
-        <v>2978</v>
+        <v>2982</v>
       </c>
       <c r="DD147" t="s">
         <v>172</v>
@@ -21497,7 +21521,7 @@
         <v>172</v>
       </c>
       <c r="DC148" t="s">
-        <v>2979</v>
+        <v>2983</v>
       </c>
       <c r="DD148" t="s">
         <v>172</v>
@@ -21523,7 +21547,7 @@
         <v>172</v>
       </c>
       <c r="DC149" t="s">
-        <v>2980</v>
+        <v>2984</v>
       </c>
       <c r="DD149" t="s">
         <v>172</v>
@@ -21549,7 +21573,7 @@
         <v>172</v>
       </c>
       <c r="DC150" t="s">
-        <v>2981</v>
+        <v>2985</v>
       </c>
       <c r="DD150" t="s">
         <v>172</v>
@@ -21575,7 +21599,7 @@
         <v>172</v>
       </c>
       <c r="DC151" t="s">
-        <v>2982</v>
+        <v>2986</v>
       </c>
       <c r="DD151" t="s">
         <v>172</v>
@@ -21601,7 +21625,7 @@
         <v>172</v>
       </c>
       <c r="DC152" t="s">
-        <v>2983</v>
+        <v>2987</v>
       </c>
       <c r="DD152" t="s">
         <v>172</v>
@@ -33456,6 +33480,48 @@
         <v>2778</v>
       </c>
       <c r="DJ918" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="919" spans="103:114">
+      <c r="CY919" t="s">
+        <v>2779</v>
+      </c>
+      <c r="CZ919" t="s">
+        <v>172</v>
+      </c>
+      <c r="DI919" t="s">
+        <v>2779</v>
+      </c>
+      <c r="DJ919" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="920" spans="103:114">
+      <c r="CY920" t="s">
+        <v>2780</v>
+      </c>
+      <c r="CZ920" t="s">
+        <v>172</v>
+      </c>
+      <c r="DI920" t="s">
+        <v>2780</v>
+      </c>
+      <c r="DJ920" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="921" spans="103:114">
+      <c r="CY921" t="s">
+        <v>2781</v>
+      </c>
+      <c r="CZ921" t="s">
+        <v>172</v>
+      </c>
+      <c r="DI921" t="s">
+        <v>2781</v>
+      </c>
+      <c r="DJ921" t="s">
         <v>172</v>
       </c>
     </row>
@@ -35131,7 +35197,7 @@
       <formula1>'Codelijsten'!$A$4:$A$5</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D9:D1000001">
       <formula1>'Codelijsten'!$C$4:$C$16</formula1>
@@ -35152,7 +35218,7 @@
       <formula1>'Codelijsten'!$M$4:$M$20</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ9:AJ1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL9:AL1000001">
       <formula1>'Codelijsten'!$O$4:$O$6</formula1>
@@ -35161,7 +35227,7 @@
       <formula1>'Codelijsten'!$Q$4:$Q$20</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW9:AW1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AY9:AY1000001">
       <formula1>'Codelijsten'!$S$4:$S$6</formula1>
@@ -35170,22 +35236,22 @@
       <formula1>'Codelijsten'!$U$4:$U$20</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BJ9:BJ1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BK9:BK1000001">
       <formula1>'Codelijsten'!$W$4:$W$7</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BN9:BN1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BO9:BO1000001">
       <formula1>'Codelijsten'!$Y$4:$Y$13</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BP9:BP1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BZ9:BZ1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CC9:CC1000001">
       <formula1>'Codelijsten'!$AA$4:$AA$17</formula1>
@@ -35200,13 +35266,13 @@
       <formula1>'Codelijsten'!$AG$4:$AG$12</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CV9:CV1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CX9:CX1000001">
       <formula1>'Codelijsten'!$AI$4:$AI$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CZ9:CZ1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DE9:DE1000001">
       <formula1>'Codelijsten'!$AK$4:$AK$60</formula1>
@@ -35907,7 +35973,7 @@
       <formula1>'Codelijsten'!$AO$4:$AO$18</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E6:E1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6:F1000001">
       <formula1>'Codelijsten'!$AQ$4:$AQ$137</formula1>
@@ -35928,7 +35994,7 @@
       <formula1>'Codelijsten'!$BA$4:$BA$9</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q6:Q1000001">
       <formula1>'Codelijsten'!$BC$4:$BC$7</formula1>
@@ -35946,13 +36012,13 @@
       <formula1>'Codelijsten'!$BK$4:$BK$11</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AR6:AR1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AT6:AT1000001">
       <formula1>'Codelijsten'!$BM$4:$BM$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV6:AV1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA6:BA1000001">
       <formula1>'Codelijsten'!$BO$4:$BO$60</formula1>
@@ -38652,7 +38718,7 @@
       <formula1>'Codelijsten'!$BQ$4:$BQ$10</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F10:F1000001">
       <formula1>'Codelijsten'!$BS$4:$BS$8</formula1>
@@ -38661,10 +38727,10 @@
       <formula1>'Codelijsten'!$BU$4:$BU$20</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N10:N1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O10:O1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P10:P1000001">
       <formula1>'Codelijsten'!$BW$4:$BW$12</formula1>
@@ -38685,19 +38751,19 @@
       <formula1>'Codelijsten'!$CG$4:$CG$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK10:AK1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AL10:AL1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM10:AM1000001">
       <formula1>'Codelijsten'!$CI$4:$CI$25</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BA10:BA1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB10:BB1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BC10:BC1000001">
       <formula1>'Codelijsten'!$CK$4:$CK$12</formula1>
@@ -38718,28 +38784,28 @@
       <formula1>'Codelijsten'!$CU$4:$CU$8</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BX10:BX1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="CU10:CU1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DK10:DK1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DS10:DS1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DU10:DU1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="DZ10:DZ1000001">
       <formula1>'Codelijsten'!$CW$4:$CW$60</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="EB10:EB1000001">
-      <formula1>'Codelijsten'!$CY$4:$CY$918</formula1>
+      <formula1>'Codelijsten'!$CY$4:$CY$921</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="EE10:EE1000001">
-      <formula1>'Codelijsten'!$DA$4:$DA$66</formula1>
+      <formula1>'Codelijsten'!$DA$4:$DA$67</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="EJ10:EJ1000001">
       <formula1>'Codelijsten'!$DC$4:$DC$152</formula1>
@@ -38751,28 +38817,28 @@
       <formula1>'Codelijsten'!$DG$4:$DG$5</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="ER10:ER1000001">
-      <formula1>'Codelijsten'!$DI$4:$DI$918</formula1>
+      <formula1>'Codelijsten'!$DI$4:$DI$921</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="EU10:EU1000001">
-      <formula1>'Codelijsten'!$DK$4:$DK$66</formula1>
+      <formula1>'Codelijsten'!$DK$4:$DK$67</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FB10:FB1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FJ10:FJ1000001">
       <formula1>'Codelijsten'!$DM$4:$DM$6</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="FY10:FY1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="GB10:GB1000001">
       <formula1>'Codelijsten'!$DO$4:$DO$12</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="GD10:GD1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="GE10:GE1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="GG10:GG1000001">
       <formula1>'Codelijsten'!$DQ$4:$DQ$6</formula1>
@@ -38885,58 +38951,58 @@
         <v>20</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>2989</v>
+        <v>2993</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>2990</v>
+        <v>2994</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2991</v>
+        <v>2995</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>2992</v>
+        <v>2996</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>2993</v>
+        <v>2997</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2994</v>
+        <v>2998</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>2995</v>
+        <v>2999</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>2996</v>
+        <v>3000</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>2997</v>
+        <v>3001</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>2999</v>
+        <v>3003</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>3000</v>
+        <v>3004</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>3001</v>
+        <v>3005</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>3002</v>
+        <v>3006</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>3003</v>
+        <v>3007</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>3004</v>
+        <v>3008</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>3006</v>
+        <v>3010</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>3007</v>
+        <v>3011</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>4</v>
@@ -38945,58 +39011,58 @@
         <v>6</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>3009</v>
+        <v>3013</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>3010</v>
+        <v>3014</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>3011</v>
+        <v>3015</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>3012</v>
+        <v>3016</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>3013</v>
+        <v>3017</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>3014</v>
+        <v>3018</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>3015</v>
+        <v>3019</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>3016</v>
+        <v>3020</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>3017</v>
+        <v>3021</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>3018</v>
+        <v>3022</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>3020</v>
+        <v>3024</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>3021</v>
+        <v>3025</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>3022</v>
+        <v>3026</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>3024</v>
+        <v>3028</v>
       </c>
       <c r="AJ1" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>3027</v>
+        <v>3031</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>3029</v>
+        <v>3033</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>3031</v>
+        <v>3035</v>
       </c>
       <c r="AN1" s="1" t="s">
         <v>152</v>
@@ -39052,7 +39118,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>2998</v>
+        <v>3002</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -39063,7 +39129,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>3008</v>
+        <v>3012</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -39078,10 +39144,10 @@
       </c>
       <c r="U2" s="1"/>
       <c r="V2" s="1" t="s">
-        <v>3009</v>
+        <v>3013</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>3019</v>
+        <v>3023</v>
       </c>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -39092,20 +39158,20 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
       <c r="AF2" s="1" t="s">
-        <v>3020</v>
+        <v>3024</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>3021</v>
+        <v>3025</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>3026</v>
+        <v>3030</v>
       </c>
       <c r="AI2" s="1"/>
       <c r="AJ2" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>3033</v>
+        <v>3037</v>
       </c>
       <c r="AL2" s="1"/>
       <c r="AM2" s="1"/>
@@ -39179,19 +39245,19 @@
       <c r="AD3" s="1"/>
       <c r="AE3" s="1"/>
       <c r="AH3" s="4" t="s">
-        <v>3023</v>
+        <v>3027</v>
       </c>
       <c r="AI3" s="4" t="s">
-        <v>3025</v>
+        <v>3029</v>
       </c>
       <c r="AK3" s="1" t="s">
-        <v>3028</v>
+        <v>3032</v>
       </c>
       <c r="AL3" s="1" t="s">
-        <v>3030</v>
+        <v>3034</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>3032</v>
+        <v>3036</v>
       </c>
       <c r="AO3" s="4" t="s">
         <v>143</v>
@@ -39359,58 +39425,58 @@
         <v>20</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>3002</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>2994</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>2995</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2996</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>2997</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>2998</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>2990</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>2991</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>2992</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>2993</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>2994</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>2995</v>
+        <v>2999</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>2996</v>
+        <v>3000</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>2997</v>
+        <v>3001</v>
       </c>
       <c r="K6" s="5" t="s">
+        <v>3012</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>3004</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>3005</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>3006</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>3007</v>
+      </c>
+      <c r="P6" s="1" t="s">
         <v>3008</v>
       </c>
-      <c r="L6" s="5" t="s">
-        <v>3000</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>3001</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>3002</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>3003</v>
-      </c>
-      <c r="P6" s="1" t="s">
-        <v>3004</v>
-      </c>
       <c r="Q6" s="1" t="s">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>3006</v>
+        <v>3010</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>3007</v>
+        <v>3011</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>4</v>
@@ -39419,58 +39485,58 @@
         <v>6</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>3009</v>
+        <v>3013</v>
       </c>
       <c r="W6" s="1" t="s">
+        <v>3023</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>3015</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>3016</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>3017</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>3018</v>
+      </c>
+      <c r="AB6" s="1" t="s">
         <v>3019</v>
       </c>
-      <c r="X6" s="1" t="s">
-        <v>3011</v>
-      </c>
-      <c r="Y6" s="1" t="s">
-        <v>3012</v>
-      </c>
-      <c r="Z6" s="1" t="s">
-        <v>3013</v>
-      </c>
-      <c r="AA6" s="1" t="s">
-        <v>3014</v>
-      </c>
-      <c r="AB6" s="1" t="s">
-        <v>3015</v>
-      </c>
       <c r="AC6" s="1" t="s">
-        <v>3016</v>
+        <v>3020</v>
       </c>
       <c r="AD6" s="1" t="s">
-        <v>3017</v>
+        <v>3021</v>
       </c>
       <c r="AE6" s="1" t="s">
-        <v>3018</v>
+        <v>3022</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>3020</v>
+        <v>3024</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>3021</v>
+        <v>3025</v>
       </c>
       <c r="AH6" s="1" t="s">
-        <v>3022</v>
+        <v>3026</v>
       </c>
       <c r="AI6" s="1" t="s">
-        <v>3024</v>
+        <v>3028</v>
       </c>
       <c r="AJ6" s="1" t="s">
         <v>153</v>
       </c>
       <c r="AK6" s="1" t="s">
-        <v>3027</v>
+        <v>3031</v>
       </c>
       <c r="AL6" s="1" t="s">
-        <v>3029</v>
+        <v>3033</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>3031</v>
+        <v>3035</v>
       </c>
       <c r="AN6" s="1" t="s">
         <v>152</v>
@@ -39546,10 +39612,10 @@
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF7:AF1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG7:AG1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AJ7:AJ1000001">
       <formula1>'Codelijsten'!$DU$4:$DU$8</formula1>
@@ -39561,10 +39627,10 @@
       <formula1>'Codelijsten'!$DY$4:$DY$27</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AU7:AU1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AW7:AW1000001">
-      <formula1>1</formula1>
+      <formula1>-146096</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="BB7:BB1000001">
       <formula1>'Codelijsten'!$EA$4:$EA$60</formula1>

</xml_diff>